<commit_message>
Added in Part 1 VHDL code. Added in VHDL interface for the new .VHD files
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29E0098-3BDD-4134-B219-5921C76C9C71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699841DC-875C-418F-AD56-E9226AE8AF45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12945" yWindow="3075" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
+    <workbookView xWindow="13650" yWindow="1740" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Log - Part 1" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="22">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -136,6 +136,18 @@
   </si>
   <si>
     <t>Unzipped the project files from Canvas. Created the folder structure as per instructions. DONE</t>
+  </si>
+  <si>
+    <t>Compared constraints for Logic Unit and Arithmetic unit to our implementations. Taking a break for dinner/supper. NOT DONE</t>
+  </si>
+  <si>
+    <t>Checked that implementation for our LogicUnit.vhd fulfills constraints. DONE</t>
+  </si>
+  <si>
+    <t>Edited ArithUnit.vhd to fulfill the constraint of adding an extra output directy from the Adder. Checked that implementation for our ArithUnit.vhd fulfills constraints. DONE</t>
+  </si>
+  <si>
+    <t>Added in VHDL interface to SLL64.vhd, SLRA64.vhd and SRL64.vhd. DONE. Taking a small break</t>
   </si>
 </sst>
 </file>
@@ -4461,7 +4473,7 @@
   <dimension ref="A1:I782"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4594,67 +4606,113 @@
     </row>
     <row r="8" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="33"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="23"/>
+      <c r="B8" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C8" s="22">
+        <v>43930</v>
+      </c>
+      <c r="D8" s="20">
+        <v>0.9</v>
+      </c>
+      <c r="E8" s="23">
+        <v>0.91319444444444453</v>
+      </c>
       <c r="F8" s="34"/>
-      <c r="G8" s="17"/>
+      <c r="G8" s="17" t="s">
+        <v>18</v>
+      </c>
       <c r="H8" s="27">
         <f t="shared" ref="H8:H71" si="1">(E8-D8)*24</f>
-        <v>0</v>
+        <v>0.31666666666666821</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="33"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="23"/>
+      <c r="B9" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C9" s="22">
+        <v>43930</v>
+      </c>
+      <c r="D9" s="20">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E9" s="23">
+        <v>0.96388888888888891</v>
+      </c>
       <c r="F9" s="34"/>
-      <c r="G9" s="17"/>
+      <c r="G9" s="17" t="s">
+        <v>19</v>
+      </c>
       <c r="H9" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.13333333333333286</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="33"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="23"/>
+      <c r="B10" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C10" s="22">
+        <v>43930</v>
+      </c>
+      <c r="D10" s="20">
+        <v>0.96388888888888891</v>
+      </c>
+      <c r="E10" s="23">
+        <v>0.97152777777777777</v>
+      </c>
       <c r="F10" s="34"/>
-      <c r="G10" s="17"/>
+      <c r="G10" s="17" t="s">
+        <v>20</v>
+      </c>
       <c r="H10" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.18333333333333268</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="33"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="23"/>
+      <c r="B11" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C11" s="22">
+        <v>43930</v>
+      </c>
+      <c r="D11" s="20">
+        <v>0.97152777777777777</v>
+      </c>
+      <c r="E11" s="23">
+        <v>0.9770833333333333</v>
+      </c>
       <c r="F11" s="34"/>
-      <c r="G11" s="17"/>
+      <c r="G11" s="17" t="s">
+        <v>21</v>
+      </c>
       <c r="H11" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.13333333333333286</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="33"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="20"/>
+      <c r="B12" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C12" s="22">
+        <v>43930</v>
+      </c>
+      <c r="D12" s="20">
+        <v>2.7083333333333334E-2</v>
+      </c>
       <c r="E12" s="23"/>
       <c r="F12" s="34"/>
       <c r="G12" s="17"/>
       <c r="H12" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-0.65</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5519,7 +5577,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>0.60000000000000053</v>
+        <v>0.71666666666666712</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Started working on barrel shifter
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699841DC-875C-418F-AD56-E9226AE8AF45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E6A3C4-20C1-43DD-93E4-B5C1F63545E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13650" yWindow="1740" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>Added in VHDL interface to SLL64.vhd, SLRA64.vhd and SRL64.vhd. DONE. Taking a small break</t>
+  </si>
+  <si>
+    <t>Started working on the 64-barrel shifters but quickly got stuck on understanding on implemnetation.</t>
+  </si>
+  <si>
+    <t>Reading the notes and trying to understand the basics of shift logical and shift arithmetic. Will try tomorrow</t>
   </si>
 </sst>
 </file>
@@ -4472,8 +4478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4702,36 +4708,54 @@
         <v>6977</v>
       </c>
       <c r="C12" s="22">
-        <v>43930</v>
+        <v>43931</v>
       </c>
       <c r="D12" s="20">
         <v>2.7083333333333334E-2</v>
       </c>
-      <c r="E12" s="23"/>
+      <c r="E12" s="23">
+        <v>7.2916666666666671E-2</v>
+      </c>
       <c r="F12" s="34"/>
-      <c r="G12" s="17"/>
+      <c r="G12" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="H12" s="27">
         <f t="shared" si="1"/>
-        <v>-0.65</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="33"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="23"/>
+      <c r="B13" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C13" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D13" s="20">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="E13" s="23">
+        <v>0.15625</v>
+      </c>
       <c r="F13" s="34"/>
-      <c r="G13" s="17"/>
+      <c r="G13" s="17" t="s">
+        <v>23</v>
+      </c>
       <c r="H13" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="33"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="22"/>
+      <c r="B14" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C14" s="22">
+        <v>43931</v>
+      </c>
       <c r="D14" s="20"/>
       <c r="E14" s="23"/>
       <c r="F14" s="34"/>
@@ -5577,7 +5601,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>0.71666666666666712</v>
+        <v>4.4666666666666668</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Begun implementation of ShiftUnit.vhd
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E6A3C4-20C1-43DD-93E4-B5C1F63545E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098A37D2-FE70-495D-A121-CE272D289E9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13650" yWindow="1740" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Log - Part 1" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Reading the notes and trying to understand the basics of shift logical and shift arithmetic. Will try tomorrow</t>
+  </si>
+  <si>
+    <t>Implemented parts of ShiftUnit.vhd. NOT DONE</t>
   </si>
 </sst>
 </file>
@@ -4479,7 +4482,7 @@
   <dimension ref="A1:I782"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4756,13 +4759,19 @@
       <c r="C14" s="22">
         <v>43931</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="23"/>
+      <c r="D14" s="20">
+        <v>0.15625</v>
+      </c>
+      <c r="E14" s="23">
+        <v>0.17361111111111113</v>
+      </c>
       <c r="F14" s="34"/>
-      <c r="G14" s="17"/>
+      <c r="G14" s="17" t="s">
+        <v>24</v>
+      </c>
       <c r="H14" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.41666666666666718</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5601,7 +5610,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>4.4666666666666668</v>
+        <v>4.8833333333333337</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Implemented most parts of ExecUnit.vhd
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098A37D2-FE70-495D-A121-CE272D289E9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B7C7B3-393C-4F35-813A-6B1509077A8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>Implemented parts of ShiftUnit.vhd. NOT DONE</t>
+  </si>
+  <si>
+    <t>Implemented most parts of ExecUnit.vhd. NOT DONE</t>
   </si>
 </sst>
 </file>
@@ -4776,15 +4779,25 @@
     </row>
     <row r="15" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="33"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="23"/>
+      <c r="B15" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C15" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D15" s="20">
+        <v>0.17361111111111113</v>
+      </c>
+      <c r="E15" s="23">
+        <v>0.19791666666666666</v>
+      </c>
       <c r="F15" s="34"/>
-      <c r="G15" s="17"/>
+      <c r="G15" s="17" t="s">
+        <v>25</v>
+      </c>
       <c r="H15" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.58333333333333259</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5610,7 +5623,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>4.8833333333333337</v>
+        <v>5.4666666666666668</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated files to version 2.3
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B7C7B3-393C-4F35-813A-6B1509077A8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C529F284-D3B7-414B-9A2A-0F9656FCD562}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>Implemented most parts of ExecUnit.vhd. NOT DONE</t>
+  </si>
+  <si>
+    <t>Reading notes to understand remaining parts of ShiftUnit.vhd and ExecUnit.vhd. Retiring for the night</t>
+  </si>
+  <si>
+    <t>Updated files to version 2.3</t>
   </si>
 </sst>
 </file>
@@ -4485,7 +4491,7 @@
   <dimension ref="A1:I782"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4802,28 +4808,48 @@
     </row>
     <row r="16" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="33"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="23"/>
+      <c r="B16" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C16" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D16" s="20">
+        <v>0.19791666666666666</v>
+      </c>
+      <c r="E16" s="23">
+        <v>0.22916666666666666</v>
+      </c>
       <c r="F16" s="34"/>
-      <c r="G16" s="17"/>
+      <c r="G16" s="17" t="s">
+        <v>26</v>
+      </c>
       <c r="H16" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="33"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="23"/>
+      <c r="B17" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C17" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D17" s="20">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="E17" s="23">
+        <v>0.90625</v>
+      </c>
       <c r="F17" s="34"/>
-      <c r="G17" s="17"/>
+      <c r="G17" s="17" t="s">
+        <v>27</v>
+      </c>
       <c r="H17" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.24999999999999911</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5623,7 +5649,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>5.4666666666666668</v>
+        <v>6.4666666666666659</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Implemented remaining code for ExecUnit.vhd and ShiftUnit.vhd
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C529F284-D3B7-414B-9A2A-0F9656FCD562}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104E6893-F3F5-4D9D-BC6C-921E5D9819C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>Updated files to version 2.3</t>
+  </si>
+  <si>
+    <t>Implemented ShiftUnit.vhd and ExecUnit.vhd. DONE</t>
+  </si>
+  <si>
+    <t>Fixed bug in ShiftUnit.vhd on not properly doing sign extension. DONE</t>
   </si>
 </sst>
 </file>
@@ -4491,7 +4497,7 @@
   <dimension ref="A1:I782"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4854,28 +4860,48 @@
     </row>
     <row r="18" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="33"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="23"/>
+      <c r="B18" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C18" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D18" s="20">
+        <v>0.90625</v>
+      </c>
+      <c r="E18" s="23">
+        <v>0.95833333333333337</v>
+      </c>
       <c r="F18" s="34"/>
-      <c r="G18" s="17"/>
+      <c r="G18" s="17" t="s">
+        <v>28</v>
+      </c>
       <c r="H18" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2500000000000009</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="33"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="23"/>
+      <c r="B19" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C19" s="22">
+        <v>43932</v>
+      </c>
+      <c r="D19" s="20">
+        <v>0.875</v>
+      </c>
+      <c r="E19" s="23">
+        <v>0.89583333333333337</v>
+      </c>
       <c r="F19" s="34"/>
-      <c r="G19" s="17"/>
+      <c r="G19" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="H19" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.50000000000000089</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5649,7 +5675,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>6.4666666666666659</v>
+        <v>8.2166666666666686</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added placeholder VHDL code
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104E6893-F3F5-4D9D-BC6C-921E5D9819C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B65139-AA35-48A4-95C6-D3DF3FC78C43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>Fixed bug in ShiftUnit.vhd on not properly doing sign extension. DONE</t>
+  </si>
+  <si>
+    <t>Added placeholder vode in Barrel Shift .vhd files to compile project.</t>
   </si>
 </sst>
 </file>
@@ -4497,7 +4500,7 @@
   <dimension ref="A1:I782"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4906,15 +4909,25 @@
     </row>
     <row r="20" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="33"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="23"/>
+      <c r="B20" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C20" s="22">
+        <v>43932</v>
+      </c>
+      <c r="D20" s="20">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="E20" s="23">
+        <v>0.90972222222222221</v>
+      </c>
       <c r="F20" s="34"/>
-      <c r="G20" s="17"/>
+      <c r="G20" s="17" t="s">
+        <v>30</v>
+      </c>
       <c r="H20" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333215</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5675,7 +5688,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>8.2166666666666686</v>
+        <v>8.5500000000000007</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed VHDL code to make it compile on ModelSim except for ShiftUnit.vhd
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B65139-AA35-48A4-95C6-D3DF3FC78C43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E8372C-2CD4-416C-9E5B-DB29A05E208B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
+    <workbookView xWindow="-12570" yWindow="2475" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Log - Part 1" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -174,7 +174,16 @@
     <t>Fixed bug in ShiftUnit.vhd on not properly doing sign extension. DONE</t>
   </si>
   <si>
-    <t>Added placeholder vode in Barrel Shift .vhd files to compile project.</t>
+    <t>Created LogicGates.vhd to hold commonly-used entities together. DONE</t>
+  </si>
+  <si>
+    <t>Added placeholder vode in Barrel Shift .vhd files to compile project. DONE</t>
+  </si>
+  <si>
+    <t>Fixed ExecUnit.vhd to make it compile on ModelSim. DONE</t>
+  </si>
+  <si>
+    <t>Fixed ShiftUnit.vhd to make it compile on ModelSim. NOT DONE. Stopping to get some food</t>
   </si>
 </sst>
 </file>
@@ -4499,8 +4508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4923,7 +4932,7 @@
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H20" s="27">
         <f t="shared" si="1"/>
@@ -4932,41 +4941,71 @@
     </row>
     <row r="21" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="33"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="23"/>
+      <c r="B21" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C21" s="22">
+        <v>43932</v>
+      </c>
+      <c r="D21" s="20">
+        <v>0.90972222222222221</v>
+      </c>
+      <c r="E21" s="23">
+        <v>0.93402777777777779</v>
+      </c>
       <c r="F21" s="34"/>
-      <c r="G21" s="17"/>
+      <c r="G21" s="17" t="s">
+        <v>30</v>
+      </c>
       <c r="H21" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.58333333333333393</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="33"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="23"/>
+      <c r="B22" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C22" s="22">
+        <v>43932</v>
+      </c>
+      <c r="D22" s="20">
+        <v>0.93402777777777779</v>
+      </c>
+      <c r="E22" s="23">
+        <v>0.96875</v>
+      </c>
       <c r="F22" s="34"/>
-      <c r="G22" s="17"/>
+      <c r="G22" s="17" t="s">
+        <v>32</v>
+      </c>
       <c r="H22" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.83333333333333304</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="33"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="23"/>
+      <c r="B23" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C23" s="22">
+        <v>43932</v>
+      </c>
+      <c r="D23" s="20">
+        <v>0.96875</v>
+      </c>
+      <c r="E23" s="23">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="F23" s="34"/>
-      <c r="G23" s="17"/>
+      <c r="G23" s="17" t="s">
+        <v>33</v>
+      </c>
       <c r="H23" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-22.75</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5688,7 +5727,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>8.5500000000000007</v>
+        <v>-12.783333333333331</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Attempted to fix ShiftUnit.vhd. Compiled on ModelSim and Quartus unsuccessfully
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E22F48-19E4-4EAD-B3D3-4F8F57B1316B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266A5467-AFE7-4B54-B9BE-3ADC662B9CA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12570" yWindow="2475" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Log - Part 1" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>Fixed ShiftUnit.vhd to make it compile on ModelSim. NOT DONE. Retiring for the day</t>
+  </si>
+  <si>
+    <t>Fixing ShiftUnit.vhd to make it compile on ModelSim. NOT DONE</t>
   </si>
 </sst>
 </file>
@@ -4509,7 +4512,7 @@
   <dimension ref="A1:I782"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5010,21 +5013,35 @@
     </row>
     <row r="24" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="33"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="23"/>
+      <c r="B24" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C24" s="22">
+        <v>43932</v>
+      </c>
+      <c r="D24" s="20">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E24" s="23">
+        <v>0.73958333333333337</v>
+      </c>
       <c r="F24" s="34"/>
-      <c r="G24" s="17"/>
+      <c r="G24" s="17" t="s">
+        <v>34</v>
+      </c>
       <c r="H24" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="33"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="22"/>
+      <c r="B25" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C25" s="22">
+        <v>43932</v>
+      </c>
       <c r="D25" s="20"/>
       <c r="E25" s="23"/>
       <c r="F25" s="34"/>
@@ -5727,7 +5744,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>-12.783333333333331</v>
+        <v>-12.033333333333331</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added SwapWord to ShiftUnit.vhd
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266A5467-AFE7-4B54-B9BE-3ADC662B9CA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D478552C-5CBD-4343-BA9B-757F15D3D483}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Fixing ShiftUnit.vhd to make it compile on ModelSim. NOT DONE</t>
+  </si>
+  <si>
+    <t>Fixing ShiftUnit.vhd with team members to make it compile on ModelSim. DONE</t>
   </si>
 </sst>
 </file>
@@ -4512,7 +4515,7 @@
   <dimension ref="A1:I782"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5042,13 +5045,19 @@
       <c r="C25" s="22">
         <v>43932</v>
       </c>
-      <c r="D25" s="20"/>
-      <c r="E25" s="23"/>
+      <c r="D25" s="20">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="E25" s="23">
+        <v>0.80208333333333337</v>
+      </c>
       <c r="F25" s="34"/>
-      <c r="G25" s="17"/>
+      <c r="G25" s="17" t="s">
+        <v>35</v>
+      </c>
       <c r="H25" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5744,7 +5753,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>-12.033333333333331</v>
+        <v>-10.533333333333331</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed SLL64.vhd of compilation errors
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D478552C-5CBD-4343-BA9B-757F15D3D483}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9921C6A-08C1-4A07-B0E3-EE2D5728C10F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>Fixing ShiftUnit.vhd with team members to make it compile on ModelSim. DONE</t>
+  </si>
+  <si>
+    <t>Fixing compilations errors with SLL64.vhd with Quartus. DONE</t>
   </si>
 </sst>
 </file>
@@ -4515,7 +4518,7 @@
   <dimension ref="A1:I782"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5003,7 +5006,7 @@
         <v>0.96875</v>
       </c>
       <c r="E23" s="23">
-        <v>2.0833333333333332E-2</v>
+        <v>0.99930555555555556</v>
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="17" t="s">
@@ -5011,7 +5014,7 @@
       </c>
       <c r="H23" s="27">
         <f t="shared" si="1"/>
-        <v>-22.75</v>
+        <v>0.73333333333333339</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5023,7 +5026,7 @@
         <v>43932</v>
       </c>
       <c r="D24" s="20">
-        <v>0.70833333333333337</v>
+        <v>0.69791666666666663</v>
       </c>
       <c r="E24" s="23">
         <v>0.73958333333333337</v>
@@ -5034,7 +5037,7 @@
       </c>
       <c r="H24" s="27">
         <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>1.0000000000000018</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5062,15 +5065,25 @@
     </row>
     <row r="26" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="33"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="23"/>
+      <c r="B26" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C26" s="22">
+        <v>43932</v>
+      </c>
+      <c r="D26" s="20">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="E26" s="23">
+        <v>0.83333333333333337</v>
+      </c>
       <c r="F26" s="34"/>
-      <c r="G26" s="17"/>
+      <c r="G26" s="17" t="s">
+        <v>36</v>
+      </c>
       <c r="H26" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5753,7 +5766,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>-10.533333333333331</v>
+        <v>13.950000000000005</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed all compilation errors on Quartus
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9921C6A-08C1-4A07-B0E3-EE2D5728C10F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F990E276-78F6-465E-8D43-39F50E655FA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
+    <workbookView xWindow="-12480" yWindow="3240" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Log - Part 1" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -192,7 +192,10 @@
     <t>Fixing ShiftUnit.vhd with team members to make it compile on ModelSim. DONE</t>
   </si>
   <si>
-    <t>Fixing compilations errors with SLL64.vhd with Quartus. DONE</t>
+    <t>Fixing compilations errors with SLL64.vhd on Quartus. DONE</t>
+  </si>
+  <si>
+    <t>Fixed compilation errors with SRL64.vhd AND sll64.vhD ON Quartus. DONE</t>
   </si>
 </sst>
 </file>
@@ -4518,7 +4521,7 @@
   <dimension ref="A1:I782"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5023,7 +5026,7 @@
         <v>6977</v>
       </c>
       <c r="C24" s="22">
-        <v>43932</v>
+        <v>43933</v>
       </c>
       <c r="D24" s="20">
         <v>0.69791666666666663</v>
@@ -5046,7 +5049,7 @@
         <v>6977</v>
       </c>
       <c r="C25" s="22">
-        <v>43932</v>
+        <v>43933</v>
       </c>
       <c r="D25" s="20">
         <v>0.73958333333333337</v>
@@ -5069,7 +5072,7 @@
         <v>6977</v>
       </c>
       <c r="C26" s="22">
-        <v>43932</v>
+        <v>43933</v>
       </c>
       <c r="D26" s="20">
         <v>0.80208333333333337</v>
@@ -5088,15 +5091,25 @@
     </row>
     <row r="27" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="33"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="23"/>
+      <c r="B27" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C27" s="22">
+        <v>43933</v>
+      </c>
+      <c r="D27" s="20">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E27" s="23">
+        <v>0.84444444444444444</v>
+      </c>
       <c r="F27" s="34"/>
-      <c r="G27" s="17"/>
+      <c r="G27" s="17" t="s">
+        <v>37</v>
+      </c>
       <c r="H27" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.26666666666666572</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5766,7 +5779,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>13.950000000000005</v>
+        <v>14.21666666666667</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Compiled successfully on Quartus and ModelSim. Updated logs
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F990E276-78F6-465E-8D43-39F50E655FA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551834C4-D9FA-4730-BA42-38FB41DF2C45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12480" yWindow="3240" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Log - Part 1" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -150,9 +150,6 @@
     <t>Added in VHDL interface to SLL64.vhd, SLRA64.vhd and SRL64.vhd. DONE. Taking a small break</t>
   </si>
   <si>
-    <t>Started working on the 64-barrel shifters but quickly got stuck on understanding on implemnetation.</t>
-  </si>
-  <si>
     <t>Reading the notes and trying to understand the basics of shift logical and shift arithmetic. Will try tomorrow</t>
   </si>
   <si>
@@ -196,6 +193,21 @@
   </si>
   <si>
     <t>Fixed compilation errors with SRL64.vhd AND sll64.vhD ON Quartus. DONE</t>
+  </si>
+  <si>
+    <t>Started working on the 64-barrel shifters but quickly got stuck on understanding on implementation</t>
+  </si>
+  <si>
+    <t>Compiled all .vhd files on ModelSim and Quartus.</t>
+  </si>
+  <si>
+    <t>Ran functional simulations for ShiftUnit.vhd. Shared results of wrong results with team members. DONE</t>
+  </si>
+  <si>
+    <t>Ran functional simulations for ExecUnit.vhd. Shared results of wrong results with team members. DONE</t>
+  </si>
+  <si>
+    <t>Committed project files and code to Github. Taking a break for supper</t>
   </si>
 </sst>
 </file>
@@ -4520,8 +4532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4760,7 +4772,7 @@
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="17" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="H12" s="27">
         <f t="shared" si="1"/>
@@ -4783,7 +4795,7 @@
       </c>
       <c r="F13" s="34"/>
       <c r="G13" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H13" s="27">
         <f t="shared" si="1"/>
@@ -4806,7 +4818,7 @@
       </c>
       <c r="F14" s="34"/>
       <c r="G14" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H14" s="27">
         <f t="shared" si="1"/>
@@ -4829,7 +4841,7 @@
       </c>
       <c r="F15" s="34"/>
       <c r="G15" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H15" s="27">
         <f t="shared" si="1"/>
@@ -4852,7 +4864,7 @@
       </c>
       <c r="F16" s="34"/>
       <c r="G16" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H16" s="27">
         <f t="shared" si="1"/>
@@ -4875,7 +4887,7 @@
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H17" s="27">
         <f t="shared" si="1"/>
@@ -4898,7 +4910,7 @@
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H18" s="27">
         <f t="shared" si="1"/>
@@ -4921,7 +4933,7 @@
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H19" s="27">
         <f t="shared" si="1"/>
@@ -4944,7 +4956,7 @@
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H20" s="27">
         <f t="shared" si="1"/>
@@ -4967,7 +4979,7 @@
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H21" s="27">
         <f t="shared" si="1"/>
@@ -4990,7 +5002,7 @@
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H22" s="27">
         <f t="shared" si="1"/>
@@ -5013,7 +5025,7 @@
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H23" s="27">
         <f t="shared" si="1"/>
@@ -5036,7 +5048,7 @@
       </c>
       <c r="F24" s="34"/>
       <c r="G24" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H24" s="27">
         <f t="shared" si="1"/>
@@ -5059,7 +5071,7 @@
       </c>
       <c r="F25" s="34"/>
       <c r="G25" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H25" s="27">
         <f t="shared" si="1"/>
@@ -5082,7 +5094,7 @@
       </c>
       <c r="F26" s="34"/>
       <c r="G26" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H26" s="27">
         <f t="shared" si="1"/>
@@ -5105,7 +5117,7 @@
       </c>
       <c r="F27" s="34"/>
       <c r="G27" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H27" s="27">
         <f t="shared" si="1"/>
@@ -5114,54 +5126,94 @@
     </row>
     <row r="28" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="33"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="23"/>
+      <c r="B28" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C28" s="22">
+        <v>43933</v>
+      </c>
+      <c r="D28" s="20">
+        <v>0.84444444444444444</v>
+      </c>
+      <c r="E28" s="23">
+        <v>0.84583333333333333</v>
+      </c>
       <c r="F28" s="34"/>
-      <c r="G28" s="17"/>
+      <c r="G28" s="17" t="s">
+        <v>38</v>
+      </c>
       <c r="H28" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.3333333333333215E-2</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="33"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="23"/>
+      <c r="B29" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C29" s="22">
+        <v>43933</v>
+      </c>
+      <c r="D29" s="20">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="E29" s="23">
+        <v>0.85069444444444453</v>
+      </c>
       <c r="F29" s="34"/>
-      <c r="G29" s="17"/>
+      <c r="G29" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="H29" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.11666666666666892</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="33"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="23"/>
+      <c r="B30" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C30" s="22">
+        <v>43933</v>
+      </c>
+      <c r="D30" s="20">
+        <v>0.85069444444444453</v>
+      </c>
+      <c r="E30" s="23">
+        <v>0.85763888888888884</v>
+      </c>
       <c r="F30" s="34"/>
-      <c r="G30" s="17"/>
+      <c r="G30" s="17" t="s">
+        <v>40</v>
+      </c>
       <c r="H30" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.16666666666666341</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="33"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="23"/>
+      <c r="B31" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C31" s="22">
+        <v>43933</v>
+      </c>
+      <c r="D31" s="20">
+        <v>0.85763888888888884</v>
+      </c>
+      <c r="E31" s="23">
+        <v>0.86111111111111116</v>
+      </c>
       <c r="F31" s="34"/>
-      <c r="G31" s="17"/>
+      <c r="G31" s="17" t="s">
+        <v>41</v>
+      </c>
       <c r="H31" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.3333333333335702E-2</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5779,7 +5831,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>14.21666666666667</v>
+        <v>14.616666666666671</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revised logs on logfile
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551834C4-D9FA-4730-BA42-38FB41DF2C45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0ECF5C-F8EF-4D7E-8524-486E616B6C1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Log - Part 1" sheetId="5" r:id="rId1"/>
-    <sheet name="Activity Log - Part 2" sheetId="4" r:id="rId2"/>
+    <sheet name="Activity Log - Part 2" sheetId="6" r:id="rId2"/>
     <sheet name="Activity Log - Part 3" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="61">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -123,58 +123,10 @@
     <t>Duration</t>
   </si>
   <si>
-    <t>Gxx</t>
-  </si>
-  <si>
     <t>Choong Jin Ng</t>
   </si>
   <si>
     <t>G47</t>
-  </si>
-  <si>
-    <t>Created empty files for all .vhd files. Created an initial draft of the report. Comitted changes to GitHub.</t>
-  </si>
-  <si>
-    <t>Unzipped the project files from Canvas. Created the folder structure as per instructions. DONE</t>
-  </si>
-  <si>
-    <t>Compared constraints for Logic Unit and Arithmetic unit to our implementations. Taking a break for dinner/supper. NOT DONE</t>
-  </si>
-  <si>
-    <t>Checked that implementation for our LogicUnit.vhd fulfills constraints. DONE</t>
-  </si>
-  <si>
-    <t>Edited ArithUnit.vhd to fulfill the constraint of adding an extra output directy from the Adder. Checked that implementation for our ArithUnit.vhd fulfills constraints. DONE</t>
-  </si>
-  <si>
-    <t>Added in VHDL interface to SLL64.vhd, SLRA64.vhd and SRL64.vhd. DONE. Taking a small break</t>
-  </si>
-  <si>
-    <t>Reading the notes and trying to understand the basics of shift logical and shift arithmetic. Will try tomorrow</t>
-  </si>
-  <si>
-    <t>Implemented parts of ShiftUnit.vhd. NOT DONE</t>
-  </si>
-  <si>
-    <t>Implemented most parts of ExecUnit.vhd. NOT DONE</t>
-  </si>
-  <si>
-    <t>Reading notes to understand remaining parts of ShiftUnit.vhd and ExecUnit.vhd. Retiring for the night</t>
-  </si>
-  <si>
-    <t>Updated files to version 2.3</t>
-  </si>
-  <si>
-    <t>Implemented ShiftUnit.vhd and ExecUnit.vhd. DONE</t>
-  </si>
-  <si>
-    <t>Fixed bug in ShiftUnit.vhd on not properly doing sign extension. DONE</t>
-  </si>
-  <si>
-    <t>Created LogicGates.vhd to hold commonly-used entities together. DONE</t>
-  </si>
-  <si>
-    <t>Added placeholder vode in Barrel Shift .vhd files to compile project. DONE</t>
   </si>
   <si>
     <t>Fixed ExecUnit.vhd to make it compile on ModelSim. DONE</t>
@@ -189,25 +141,130 @@
     <t>Fixing ShiftUnit.vhd with team members to make it compile on ModelSim. DONE</t>
   </si>
   <si>
-    <t>Fixing compilations errors with SLL64.vhd on Quartus. DONE</t>
+    <t>Compared constraints for LogicUnit to our implementations. Taking a break for dinner/supper - NOT DONE</t>
   </si>
   <si>
-    <t>Fixed compilation errors with SRL64.vhd AND sll64.vhD ON Quartus. DONE</t>
+    <t>Resume comparing constraints for LogicUnit to our implementations. - DONE</t>
   </si>
   <si>
-    <t>Started working on the 64-barrel shifters but quickly got stuck on understanding on implementation</t>
+    <t>Created empty files for all .vhd files. Created an initial draft of the report. Made first commit to GitHub. -DONE</t>
   </si>
   <si>
-    <t>Compiled all .vhd files on ModelSim and Quartus.</t>
+    <t>Unzipped the project files from Canvas. Created the folder structure as per instructions. -DONE</t>
   </si>
   <si>
-    <t>Ran functional simulations for ShiftUnit.vhd. Shared results of wrong results with team members. DONE</t>
+    <t>Compared constraints for Arithmetic unit to our implementations. Taking a break for dinner/supper - DONE</t>
   </si>
   <si>
-    <t>Ran functional simulations for ExecUnit.vhd. Shared results of wrong results with team members. DONE</t>
+    <t>Edited ArithUnit.vhd to fulfill the constraint of adding an extra output directy from the Adder - DONE</t>
   </si>
   <si>
-    <t>Committed project files and code to Github. Taking a break for supper</t>
+    <t>Final runthrough that implementation of ArithUnit complies with constraints. - DONE</t>
+  </si>
+  <si>
+    <t>Added VHDL interface and entity declaration to SLL64.vhd, SLRA64.vhd and SRL64.vhd. Taking a small break to join a friend in a game. -DONEW</t>
+  </si>
+  <si>
+    <t>Read specifications for barrel shifters. -DONE</t>
+  </si>
+  <si>
+    <t>Started working on the 64-barrel shifters but got stuck on understanding on implementation. -NOT DONE</t>
+  </si>
+  <si>
+    <t>Added VHDL interface and entity declaration for ShiftUnit.vhd. Added signals for architecture for ShiftUnit.vhd. -DONE</t>
+  </si>
+  <si>
+    <t>Added the multiplexers and the wiring logic for them. Left comments on some of the wires to remind myself to ask for help from team members tomorrow. -NOT DONE</t>
+  </si>
+  <si>
+    <t>Added VHDL interface and entity declaration for ExecUnit.vhd. Added signals for architecture for ShiftUnit.vhd. -DONE</t>
+  </si>
+  <si>
+    <t>Added the entities ArithUnit, ShiftUnit, LogicUnit to ExecUnit.vhd. -DONE</t>
+  </si>
+  <si>
+    <t>Started working on the multiplexer to select the results for the output. Wired the ShiftUnit's and LogicUnit's result but was unsure on the other input wires. -NOT DONE</t>
+  </si>
+  <si>
+    <t>Updated all project files to version 2.3. -DONE</t>
+  </si>
+  <si>
+    <t>Implemented remaining work on ShiftUnit's multiplexers. - DONE</t>
+  </si>
+  <si>
+    <t>Implemented remaining work on AltB and AltBu MUX input signals. - DONE</t>
+  </si>
+  <si>
+    <t>Read notes on the Execution Unit. Asked friends on best practice to implement the AltB and AltBu MUX input signals for ExecUnit.vhd. Pushed changes to GitHub and then retired for the night -NOT DONE</t>
+  </si>
+  <si>
+    <t>Tried to compile on ModelSim to find all compilation errors for ShiftUnit.vhd, ArithUnit.vhd, ExecUnit.vhd and LogicUnit.vhd. -DONE</t>
+  </si>
+  <si>
+    <t>Read notes on how to build a proper barrel shifter for shifting logical and shifting right arithmetic. Got very tired and decided to work on this tomorrow. Updated team members on progress. -NOT DONE</t>
+  </si>
+  <si>
+    <t>Fixed obvious compilation errors on ModelSim as best as possbile. Rest of compilation errors will be dealt with tomorrow. Pushed changes before going to sleep. -NOT DONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed </t>
+  </si>
+  <si>
+    <t>Added placeholder code into barrel shifter .vhd files to compile project on ModelSim. -DONE</t>
+  </si>
+  <si>
+    <t>Created LogicGates.vhd to hold commonly-used entities. -DONE</t>
+  </si>
+  <si>
+    <t>Fixed bug in ShiftUnit.vhd on not properly doing sign extension. -DONE</t>
+  </si>
+  <si>
+    <t>Tried to compile on ModelSim to find all compilation errors for all .vhd files. - DONE</t>
+  </si>
+  <si>
+    <t>Fixed ShiftUnit.vhd as it does not swap the lower 32 bits of A to the upper 32 bits. -DONE</t>
+  </si>
+  <si>
+    <t>Tried to compile on Quartus. Lots of compilation errors on the barrel shifters.</t>
+  </si>
+  <si>
+    <t>Fixing compilations errors with SLL64.vhd on Quartus. Communicated changes to team members and waiting on feedback. -DONE</t>
+  </si>
+  <si>
+    <t>Fixing compilations errors with SRL64.vhd and SLL64 on Quartus. Communicated changes to team members and waiting on feedback. -DONE</t>
+  </si>
+  <si>
+    <t>Compiled all .vhd files on ModelSim and Quartus to make sure everything is compilable. -DONE</t>
+  </si>
+  <si>
+    <t>Ran functional simulations for ShiftUnit.vhd. Shared results of wrong results with team members. -DONE</t>
+  </si>
+  <si>
+    <t>Ran functional simulations for ExecUnit.vhd. Shared results of wrong results with team members. -DONE</t>
+  </si>
+  <si>
+    <t>Ran functional simulations for ArithUnit and LogicUnit.vhd. Results are still good. -DONE</t>
+  </si>
+  <si>
+    <t>Pushed changes to GitHub. Stopping work on project to focus on another course's final exam in a few days. Communicated changes and progress to team members. -DONE</t>
+  </si>
+  <si>
+    <t>As per team members' suggestion, created a Google Docs file to collaborate on document content concurrnetly rather than fixing merge conflicts upon pushing/pulling changes top .doc file. - DONE</t>
+  </si>
+  <si>
+    <t>Asked team members on progress to be briefed on what needs to be done so that I can work on it when I am available. -DONE</t>
+  </si>
+  <si>
+    <t>Fixed Part 2 logs as per feedback from part 1. -DONE</t>
+  </si>
+  <si>
+    <t>Added incontent from part 1 into Google Doc file. Returned back to other assignments - DONE</t>
+  </si>
+  <si>
+    <t>Read feedback comments from part 1. -DONE</t>
+  </si>
+  <si>
+    <t>Pulled changes from Github to go over changes team members have made in the past few days. -DONE</t>
   </si>
 </sst>
 </file>
@@ -516,7 +573,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -653,6 +710,9 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,6 +765,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1006,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090E6E40-83BD-4CBB-97D3-102021CD8368}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,7 +1091,9 @@
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="37" t="s">
+        <v>13</v>
+      </c>
       <c r="C1" s="37"/>
       <c r="D1" s="37"/>
       <c r="E1" s="38" t="s">
@@ -1040,7 +1106,9 @@
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="39"/>
+      <c r="B2" s="39">
+        <v>301226977</v>
+      </c>
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
       <c r="E2" s="38"/>
@@ -1052,7 +1120,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="40"/>
       <c r="D3" s="40"/>
@@ -2766,11 +2834,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD091BD6-3364-44DE-8BB4-985458F62AD8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5014613-EBCB-42CE-9E22-81901AAC5CBA}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2790,7 +2858,9 @@
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="37" t="s">
+        <v>13</v>
+      </c>
       <c r="C1" s="37"/>
       <c r="D1" s="37"/>
       <c r="E1" s="38" t="s">
@@ -2803,7 +2873,9 @@
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="39"/>
+      <c r="B2" s="39">
+        <v>301226977</v>
+      </c>
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
       <c r="E2" s="38"/>
@@ -2815,7 +2887,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="40"/>
       <c r="D3" s="40"/>
@@ -2852,601 +2924,1061 @@
     </row>
     <row r="6" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21"/>
+      <c r="B6" s="13">
+        <v>6977</v>
+      </c>
+      <c r="C6" s="19">
+        <v>43930</v>
+      </c>
+      <c r="D6" s="20">
+        <v>0.875</v>
+      </c>
+      <c r="E6" s="21">
+        <v>0.89583333333333337</v>
+      </c>
       <c r="F6" s="32"/>
-      <c r="G6" s="16"/>
+      <c r="G6" s="16" t="s">
+        <v>22</v>
+      </c>
       <c r="H6" s="12">
-        <f t="shared" ref="H6" si="0">(E6-D6)*24</f>
-        <v>0</v>
+        <f t="shared" ref="H6:H69" si="0">(E6-D6)*24</f>
+        <v>0.50000000000000089</v>
       </c>
       <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="23"/>
+      <c r="B7" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C7" s="22">
+        <v>43930</v>
+      </c>
+      <c r="D7" s="20">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="E7" s="23">
+        <v>0.9</v>
+      </c>
       <c r="F7" s="34"/>
-      <c r="G7" s="17"/>
+      <c r="G7" s="17" t="s">
+        <v>21</v>
+      </c>
       <c r="H7" s="27">
-        <f>(E7-D7)*24</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>9.9999999999999645E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="33"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="23"/>
+      <c r="B8" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C8" s="22">
+        <v>43930</v>
+      </c>
+      <c r="D8" s="20">
+        <v>0.9</v>
+      </c>
+      <c r="E8" s="23">
+        <v>0.90972222222222221</v>
+      </c>
       <c r="F8" s="34"/>
-      <c r="G8" s="17"/>
+      <c r="G8" s="17" t="s">
+        <v>23</v>
+      </c>
       <c r="H8" s="27">
-        <f t="shared" ref="H8:H71" si="1">(E8-D8)*24</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.2333333333333325</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="33"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="23"/>
+      <c r="B9" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C9" s="22">
+        <v>43930</v>
+      </c>
+      <c r="D9" s="20">
+        <v>0.90972222222222221</v>
+      </c>
+      <c r="E9" s="23">
+        <v>0.91527777777777775</v>
+      </c>
       <c r="F9" s="34"/>
-      <c r="G9" s="17"/>
+      <c r="G9" s="17" t="s">
+        <v>19</v>
+      </c>
       <c r="H9" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.13333333333333286</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="33"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="23"/>
+      <c r="B10" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C10" s="22">
+        <v>43930</v>
+      </c>
+      <c r="D10" s="20">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E10" s="23">
+        <v>0.96388888888888891</v>
+      </c>
       <c r="F10" s="34"/>
-      <c r="G10" s="17"/>
+      <c r="G10" s="17" t="s">
+        <v>20</v>
+      </c>
       <c r="H10" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.13333333333333286</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="33"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="23"/>
+      <c r="B11" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C11" s="22">
+        <v>43930</v>
+      </c>
+      <c r="D11" s="20">
+        <v>0.96388888888888891</v>
+      </c>
+      <c r="E11" s="23">
+        <v>0.96875</v>
+      </c>
       <c r="F11" s="34"/>
-      <c r="G11" s="17"/>
+      <c r="G11" s="17" t="s">
+        <v>24</v>
+      </c>
       <c r="H11" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.11666666666666625</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="33"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="23"/>
+      <c r="B12" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C12" s="22">
+        <v>43930</v>
+      </c>
+      <c r="D12" s="20">
+        <v>0.96875</v>
+      </c>
+      <c r="E12" s="23">
+        <v>0.97152777777777777</v>
+      </c>
       <c r="F12" s="34"/>
-      <c r="G12" s="17"/>
+      <c r="G12" s="17" t="s">
+        <v>25</v>
+      </c>
       <c r="H12" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>6.666666666666643E-2</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="33"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="23"/>
+      <c r="B13" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C13" s="22">
+        <v>43930</v>
+      </c>
+      <c r="D13" s="20">
+        <v>0.97152777777777777</v>
+      </c>
+      <c r="E13" s="23">
+        <v>0.9770833333333333</v>
+      </c>
       <c r="F13" s="34"/>
-      <c r="G13" s="17"/>
+      <c r="G13" s="17" t="s">
+        <v>26</v>
+      </c>
       <c r="H13" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.13333333333333286</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="33"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="23"/>
+      <c r="B14" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C14" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D14" s="23">
+        <v>0.52430555555555558</v>
+      </c>
+      <c r="E14" s="23">
+        <v>0.52777777777777779</v>
+      </c>
       <c r="F14" s="34"/>
-      <c r="G14" s="17"/>
+      <c r="G14" s="17" t="s">
+        <v>27</v>
+      </c>
       <c r="H14" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>8.3333333333333037E-2</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="33"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="23"/>
+      <c r="B15" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C15" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D15" s="20">
+        <v>2.7083333333333334E-2</v>
+      </c>
+      <c r="E15" s="23">
+        <v>7.2916666666666671E-2</v>
+      </c>
       <c r="F15" s="34"/>
-      <c r="G15" s="17"/>
+      <c r="G15" s="17" t="s">
+        <v>28</v>
+      </c>
       <c r="H15" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="33"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="23"/>
+      <c r="B16" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C16" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D16" s="20">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="E16" s="23">
+        <v>0.15625</v>
+      </c>
       <c r="F16" s="34"/>
-      <c r="G16" s="17"/>
+      <c r="G16" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="H16" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="33"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="23"/>
+      <c r="B17" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C17" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D17" s="20">
+        <v>0.15625</v>
+      </c>
+      <c r="E17" s="23">
+        <v>0.15972222222222224</v>
+      </c>
       <c r="F17" s="34"/>
-      <c r="G17" s="17"/>
+      <c r="G17" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="H17" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>8.3333333333333703E-2</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="33"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="23"/>
+      <c r="B18" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C18" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D18" s="20">
+        <v>0.15972222222222224</v>
+      </c>
+      <c r="E18" s="23">
+        <v>0.17708333333333334</v>
+      </c>
       <c r="F18" s="34"/>
-      <c r="G18" s="17"/>
+      <c r="G18" s="17" t="s">
+        <v>30</v>
+      </c>
       <c r="H18" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.41666666666666652</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="33"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="23"/>
+      <c r="B19" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C19" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D19" s="20">
+        <v>0.17708333333333334</v>
+      </c>
+      <c r="E19" s="23">
+        <v>0.18402777777777779</v>
+      </c>
       <c r="F19" s="34"/>
-      <c r="G19" s="17"/>
+      <c r="G19" s="17" t="s">
+        <v>31</v>
+      </c>
       <c r="H19" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.16666666666666674</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="33"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="23"/>
+      <c r="B20" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C20" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D20" s="20">
+        <v>0.18402777777777779</v>
+      </c>
+      <c r="E20" s="23">
+        <v>0.19791666666666666</v>
+      </c>
       <c r="F20" s="34"/>
-      <c r="G20" s="17"/>
+      <c r="G20" s="17" t="s">
+        <v>32</v>
+      </c>
       <c r="H20" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.33333333333333282</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="33"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="23"/>
+      <c r="B21" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C21" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D21" s="20">
+        <v>0.19791666666666666</v>
+      </c>
+      <c r="E21" s="23">
+        <v>0.20486111111111113</v>
+      </c>
       <c r="F21" s="34"/>
-      <c r="G21" s="17"/>
+      <c r="G21" s="17" t="s">
+        <v>33</v>
+      </c>
       <c r="H21" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.16666666666666741</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="33"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="23"/>
+      <c r="B22" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C22" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D22" s="20">
+        <v>0.20486111111111113</v>
+      </c>
+      <c r="E22" s="23">
+        <v>0.22569444444444445</v>
+      </c>
       <c r="F22" s="34"/>
-      <c r="G22" s="17"/>
+      <c r="G22" s="17" t="s">
+        <v>37</v>
+      </c>
       <c r="H22" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.49999999999999956</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="33"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="23"/>
+      <c r="B23" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C23" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D23" s="20">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="E23" s="23">
+        <v>0.91319444444444453</v>
+      </c>
       <c r="F23" s="34"/>
-      <c r="G23" s="17"/>
+      <c r="G23" s="17" t="s">
+        <v>34</v>
+      </c>
       <c r="H23" s="27">
         <f>(E23-D23)*24</f>
-        <v>0</v>
+        <v>0.41666666666666785</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="33"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="23"/>
+      <c r="B24" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C24" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D24" s="20">
+        <v>0.91319444444444453</v>
+      </c>
+      <c r="E24" s="23">
+        <v>0.9375</v>
+      </c>
       <c r="F24" s="34"/>
-      <c r="G24" s="17"/>
+      <c r="G24" s="17" t="s">
+        <v>35</v>
+      </c>
       <c r="H24" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.58333333333333126</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="33"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="23"/>
+      <c r="B25" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C25" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D25" s="20">
+        <v>0.9375</v>
+      </c>
+      <c r="E25" s="23">
+        <v>0.95833333333333337</v>
+      </c>
       <c r="F25" s="34"/>
-      <c r="G25" s="17"/>
+      <c r="G25" s="17" t="s">
+        <v>36</v>
+      </c>
       <c r="H25" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.50000000000000089</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="33"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="23"/>
+      <c r="B26" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C26" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D26" s="20">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E26" s="23">
+        <v>0.96527777777777779</v>
+      </c>
       <c r="F26" s="34"/>
-      <c r="G26" s="17"/>
+      <c r="G26" s="17" t="s">
+        <v>38</v>
+      </c>
       <c r="H26" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.16666666666666607</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="33"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="23"/>
+      <c r="B27" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C27" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D27" s="20">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E27" s="23">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="F27" s="34"/>
-      <c r="G27" s="17"/>
+      <c r="G27" s="17" t="s">
+        <v>40</v>
+      </c>
       <c r="H27" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.33333333333333215</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="33"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="23"/>
+      <c r="B28" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C28" s="22">
+        <v>43932</v>
+      </c>
+      <c r="D28" s="20">
+        <v>0.875</v>
+      </c>
+      <c r="E28" s="23">
+        <v>0.89583333333333337</v>
+      </c>
       <c r="F28" s="34"/>
-      <c r="G28" s="17"/>
+      <c r="G28" s="17" t="s">
+        <v>44</v>
+      </c>
       <c r="H28" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.50000000000000089</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="33"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="23"/>
+      <c r="B29" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C29" s="22">
+        <v>43932</v>
+      </c>
+      <c r="D29" s="23">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="E29" s="23">
+        <v>0.90972222222222221</v>
+      </c>
       <c r="F29" s="34"/>
-      <c r="G29" s="17"/>
+      <c r="G29" s="17" t="s">
+        <v>41</v>
+      </c>
       <c r="H29" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.33333333333333215</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="33"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="23"/>
+      <c r="B30" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C30" s="22">
+        <v>43932</v>
+      </c>
+      <c r="D30" s="20">
+        <v>0.90972222222222221</v>
+      </c>
+      <c r="E30" s="23">
+        <v>0.92361111111111116</v>
+      </c>
       <c r="F30" s="34"/>
-      <c r="G30" s="17"/>
+      <c r="G30" s="17" t="s">
+        <v>42</v>
+      </c>
       <c r="H30" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.33333333333333481</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="33"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="23"/>
+      <c r="B31" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C31" s="22">
+        <v>43932</v>
+      </c>
+      <c r="D31" s="20">
+        <v>0.92361111111111116</v>
+      </c>
+      <c r="E31" s="23">
+        <v>0.9375</v>
+      </c>
       <c r="F31" s="34"/>
-      <c r="G31" s="17"/>
+      <c r="G31" s="17" t="s">
+        <v>43</v>
+      </c>
       <c r="H31" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.33333333333333215</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="33"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="23"/>
+      <c r="B32" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C32" s="22">
+        <v>43932</v>
+      </c>
+      <c r="D32" s="20">
+        <v>0.9375</v>
+      </c>
+      <c r="E32" s="23">
+        <v>0.94097222222222221</v>
+      </c>
       <c r="F32" s="34"/>
-      <c r="G32" s="17"/>
+      <c r="G32" s="17" t="s">
+        <v>45</v>
+      </c>
       <c r="H32" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>8.3333333333333037E-2</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="33"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="23"/>
+      <c r="B33" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C33" s="22">
+        <v>43932</v>
+      </c>
+      <c r="D33" s="20">
+        <v>0.94097222222222221</v>
+      </c>
+      <c r="E33" s="23">
+        <v>0.96875</v>
+      </c>
       <c r="F33" s="34"/>
-      <c r="G33" s="17"/>
+      <c r="G33" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="H33" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.66666666666666696</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="33"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="23"/>
+      <c r="B34" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C34" s="22">
+        <v>43932</v>
+      </c>
+      <c r="D34" s="20">
+        <v>0.96875</v>
+      </c>
+      <c r="E34" s="23">
+        <v>0.99930555555555556</v>
+      </c>
       <c r="F34" s="34"/>
-      <c r="G34" s="17"/>
+      <c r="G34" s="17" t="s">
+        <v>16</v>
+      </c>
       <c r="H34" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.73333333333333339</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="33"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="23"/>
+      <c r="B35" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C35" s="22">
+        <v>43933</v>
+      </c>
+      <c r="D35" s="20">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="E35" s="23">
+        <v>0.73958333333333337</v>
+      </c>
       <c r="F35" s="34"/>
-      <c r="G35" s="17"/>
+      <c r="G35" s="17" t="s">
+        <v>17</v>
+      </c>
       <c r="H35" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.0000000000000018</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="33"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="23"/>
+      <c r="B36" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C36" s="22">
+        <v>43933</v>
+      </c>
+      <c r="D36" s="20">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="E36" s="23">
+        <v>0.76388888888888884</v>
+      </c>
       <c r="F36" s="34"/>
-      <c r="G36" s="17"/>
+      <c r="G36" s="17" t="s">
+        <v>46</v>
+      </c>
       <c r="H36" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.58333333333333126</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="33"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="23"/>
+      <c r="B37" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C37" s="22">
+        <v>43933</v>
+      </c>
+      <c r="D37" s="20">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="E37" s="23">
+        <v>0.80208333333333337</v>
+      </c>
       <c r="F37" s="34"/>
-      <c r="G37" s="17"/>
+      <c r="G37" s="17" t="s">
+        <v>18</v>
+      </c>
       <c r="H37" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.91666666666666874</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="33"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="23"/>
+      <c r="B38" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C38" s="22">
+        <v>43933</v>
+      </c>
+      <c r="D38" s="20">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="E38" s="23">
+        <v>0.80902777777777779</v>
+      </c>
       <c r="F38" s="34"/>
-      <c r="G38" s="17"/>
+      <c r="G38" s="17" t="s">
+        <v>47</v>
+      </c>
       <c r="H38" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.16666666666666607</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="33"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="23"/>
+      <c r="B39" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C39" s="22">
+        <v>43933</v>
+      </c>
+      <c r="D39" s="20">
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="E39" s="23">
+        <v>0.83333333333333337</v>
+      </c>
       <c r="F39" s="34"/>
-      <c r="G39" s="17"/>
+      <c r="G39" s="17" t="s">
+        <v>48</v>
+      </c>
       <c r="H39" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.58333333333333393</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="33"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="23"/>
+      <c r="B40" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C40" s="22">
+        <v>43933</v>
+      </c>
+      <c r="D40" s="20">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E40" s="23">
+        <v>0.84375</v>
+      </c>
       <c r="F40" s="34"/>
-      <c r="G40" s="17"/>
+      <c r="G40" s="17" t="s">
+        <v>49</v>
+      </c>
       <c r="H40" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.24999999999999911</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="33"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="23"/>
+      <c r="B41" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C41" s="22">
+        <v>43933</v>
+      </c>
+      <c r="D41" s="20">
+        <v>0.84444444444444444</v>
+      </c>
+      <c r="E41" s="23">
+        <v>0.84583333333333333</v>
+      </c>
       <c r="F41" s="34"/>
-      <c r="G41" s="17"/>
+      <c r="G41" s="17" t="s">
+        <v>50</v>
+      </c>
       <c r="H41" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.3333333333333215E-2</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="33"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="23"/>
+      <c r="B42" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C42" s="22">
+        <v>43933</v>
+      </c>
+      <c r="D42" s="20">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="E42" s="23">
+        <v>0.85069444444444453</v>
+      </c>
       <c r="F42" s="34"/>
-      <c r="G42" s="17"/>
+      <c r="G42" s="17" t="s">
+        <v>51</v>
+      </c>
       <c r="H42" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.11666666666666892</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="33"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="23"/>
+      <c r="B43" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C43" s="22">
+        <v>43933</v>
+      </c>
+      <c r="D43" s="20">
+        <v>0.85069444444444453</v>
+      </c>
+      <c r="E43" s="23">
+        <v>0.85763888888888884</v>
+      </c>
       <c r="F43" s="34"/>
-      <c r="G43" s="17"/>
+      <c r="G43" s="17" t="s">
+        <v>52</v>
+      </c>
       <c r="H43" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.16666666666666341</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="33"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="23"/>
+      <c r="B44" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C44" s="22">
+        <v>43933</v>
+      </c>
+      <c r="D44" s="20">
+        <v>0.85763888888888884</v>
+      </c>
+      <c r="E44" s="23">
+        <v>0.86458333333333337</v>
+      </c>
       <c r="F44" s="34"/>
-      <c r="G44" s="17"/>
+      <c r="G44" s="17" t="s">
+        <v>53</v>
+      </c>
       <c r="H44" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.16666666666666874</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="33"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="22"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="23"/>
+      <c r="B45" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C45" s="22">
+        <v>43933</v>
+      </c>
+      <c r="D45" s="20">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="E45" s="23">
+        <v>0.86805555555555547</v>
+      </c>
       <c r="F45" s="34"/>
-      <c r="G45" s="17"/>
+      <c r="G45" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="H45" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>8.3333333333330373E-2</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="33"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="22"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="23"/>
+      <c r="B46" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C46" s="22">
+        <v>43936</v>
+      </c>
+      <c r="D46" s="20">
+        <v>0.89236111111111116</v>
+      </c>
+      <c r="E46" s="23">
+        <v>0.89583333333333337</v>
+      </c>
       <c r="F46" s="34"/>
-      <c r="G46" s="17"/>
+      <c r="G46" s="17" t="s">
+        <v>56</v>
+      </c>
       <c r="H46" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>8.3333333333333037E-2</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="33"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="22"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="23"/>
+      <c r="B47" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C47" s="22">
+        <v>43936</v>
+      </c>
+      <c r="D47" s="20">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="E47" s="23">
+        <v>0.89930555555555547</v>
+      </c>
       <c r="F47" s="34"/>
-      <c r="G47" s="17"/>
+      <c r="G47" s="17" t="s">
+        <v>55</v>
+      </c>
       <c r="H47" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>8.3333333333330373E-2</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="33"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="22"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="23"/>
+      <c r="B48" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C48" s="22">
+        <v>43936</v>
+      </c>
+      <c r="D48" s="20">
+        <v>0.89930555555555547</v>
+      </c>
+      <c r="E48" s="23">
+        <v>0.90625</v>
+      </c>
       <c r="F48" s="34"/>
-      <c r="G48" s="17"/>
+      <c r="G48" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="H48" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.16666666666666874</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="33"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="22"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="23"/>
+      <c r="B49" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C49" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D49" s="20">
+        <v>0.17013888888888887</v>
+      </c>
+      <c r="E49" s="23">
+        <v>0.17500000000000002</v>
+      </c>
       <c r="F49" s="34"/>
-      <c r="G49" s="17"/>
+      <c r="G49" s="17" t="s">
+        <v>59</v>
+      </c>
       <c r="H49" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.11666666666666758</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="33"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="22"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="23"/>
+      <c r="B50" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C50" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D50" s="20">
+        <v>0.17500000000000002</v>
+      </c>
+      <c r="E50" s="23">
+        <v>0.21111111111111111</v>
+      </c>
       <c r="F50" s="34"/>
-      <c r="G50" s="17"/>
+      <c r="G50" s="17" t="s">
+        <v>57</v>
+      </c>
       <c r="H50" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.86666666666666625</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="33"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="22"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="23"/>
+      <c r="B51" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C51" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D51" s="20">
+        <v>0.21111111111111111</v>
+      </c>
+      <c r="E51" s="23">
+        <v>0.21527777777777779</v>
+      </c>
       <c r="F51" s="34"/>
-      <c r="G51" s="17"/>
+      <c r="G51" s="17" t="s">
+        <v>60</v>
+      </c>
       <c r="H51" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.10000000000000031</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3458,7 +3990,7 @@
       <c r="F52" s="34"/>
       <c r="G52" s="17"/>
       <c r="H52" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3471,7 +4003,7 @@
       <c r="F53" s="34"/>
       <c r="G53" s="17"/>
       <c r="H53" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3484,7 +4016,7 @@
       <c r="F54" s="34"/>
       <c r="G54" s="17"/>
       <c r="H54" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3497,7 +4029,7 @@
       <c r="F55" s="34"/>
       <c r="G55" s="17"/>
       <c r="H55" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3510,7 +4042,7 @@
       <c r="F56" s="34"/>
       <c r="G56" s="17"/>
       <c r="H56" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3523,7 +4055,7 @@
       <c r="F57" s="34"/>
       <c r="G57" s="17"/>
       <c r="H57" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3536,7 +4068,7 @@
       <c r="F58" s="34"/>
       <c r="G58" s="17"/>
       <c r="H58" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3549,7 +4081,7 @@
       <c r="F59" s="34"/>
       <c r="G59" s="17"/>
       <c r="H59" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3562,7 +4094,7 @@
       <c r="F60" s="34"/>
       <c r="G60" s="17"/>
       <c r="H60" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3575,7 +4107,7 @@
       <c r="F61" s="34"/>
       <c r="G61" s="17"/>
       <c r="H61" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3588,7 +4120,7 @@
       <c r="F62" s="34"/>
       <c r="G62" s="17"/>
       <c r="H62" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3601,7 +4133,7 @@
       <c r="F63" s="34"/>
       <c r="G63" s="17"/>
       <c r="H63" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3614,7 +4146,7 @@
       <c r="F64" s="34"/>
       <c r="G64" s="17"/>
       <c r="H64" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3627,7 +4159,7 @@
       <c r="F65" s="34"/>
       <c r="G65" s="17"/>
       <c r="H65" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3640,7 +4172,7 @@
       <c r="F66" s="34"/>
       <c r="G66" s="17"/>
       <c r="H66" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3653,7 +4185,7 @@
       <c r="F67" s="34"/>
       <c r="G67" s="17"/>
       <c r="H67" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3666,7 +4198,7 @@
       <c r="F68" s="34"/>
       <c r="G68" s="17"/>
       <c r="H68" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3679,7 +4211,7 @@
       <c r="F69" s="34"/>
       <c r="G69" s="17"/>
       <c r="H69" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3692,7 +4224,7 @@
       <c r="F70" s="34"/>
       <c r="G70" s="17"/>
       <c r="H70" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H70:H129" si="1">(E70-D70)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -3718,7 +4250,7 @@
       <c r="F72" s="34"/>
       <c r="G72" s="17"/>
       <c r="H72" s="27">
-        <f t="shared" ref="H72:H78" si="2">(E72-D72)*24</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3731,7 +4263,7 @@
       <c r="F73" s="34"/>
       <c r="G73" s="17"/>
       <c r="H73" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3744,7 +4276,7 @@
       <c r="F74" s="34"/>
       <c r="G74" s="17"/>
       <c r="H74" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3757,7 +4289,7 @@
       <c r="F75" s="34"/>
       <c r="G75" s="17"/>
       <c r="H75" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3770,7 +4302,7 @@
       <c r="F76" s="34"/>
       <c r="G76" s="17"/>
       <c r="H76" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3783,7 +4315,7 @@
       <c r="F77" s="34"/>
       <c r="G77" s="17"/>
       <c r="H77" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3796,15 +4328,15 @@
       <c r="F78" s="36"/>
       <c r="G78" s="18"/>
       <c r="H78" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F79" s="30"/>
+      <c r="F79" s="41"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>0</v>
+        <v>16.733333333333334</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4519,7 +5051,7 @@
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="H6:H78">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4532,8 +5064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4554,7 +5086,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="37"/>
       <c r="D1" s="37"/>
@@ -4582,7 +5114,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="40"/>
       <c r="D3" s="40"/>
@@ -4619,601 +5151,341 @@
     </row>
     <row r="6" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
-      <c r="B6" s="13">
-        <v>6977</v>
-      </c>
-      <c r="C6" s="19">
-        <v>43930</v>
-      </c>
-      <c r="D6" s="20">
-        <v>0.875</v>
-      </c>
-      <c r="E6" s="21">
-        <v>0.89583333333333337</v>
-      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="21"/>
       <c r="F6" s="32"/>
-      <c r="G6" s="16" t="s">
-        <v>17</v>
-      </c>
+      <c r="G6" s="16"/>
       <c r="H6" s="12">
         <f t="shared" ref="H6" si="0">(E6-D6)*24</f>
-        <v>0.50000000000000089</v>
+        <v>0</v>
       </c>
       <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33"/>
-      <c r="B7" s="14">
-        <v>6977</v>
-      </c>
-      <c r="C7" s="22">
-        <v>43930</v>
-      </c>
-      <c r="D7" s="20">
-        <v>0.89583333333333337</v>
-      </c>
-      <c r="E7" s="23">
-        <v>0.9</v>
-      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="23"/>
       <c r="F7" s="34"/>
-      <c r="G7" s="17" t="s">
-        <v>16</v>
-      </c>
+      <c r="G7" s="17"/>
       <c r="H7" s="27">
         <f>(E7-D7)*24</f>
-        <v>9.9999999999999645E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="33"/>
-      <c r="B8" s="14">
-        <v>6977</v>
-      </c>
-      <c r="C8" s="22">
-        <v>43930</v>
-      </c>
-      <c r="D8" s="20">
-        <v>0.9</v>
-      </c>
-      <c r="E8" s="23">
-        <v>0.91319444444444453</v>
-      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="23"/>
       <c r="F8" s="34"/>
-      <c r="G8" s="17" t="s">
-        <v>18</v>
-      </c>
+      <c r="G8" s="17"/>
       <c r="H8" s="27">
         <f t="shared" ref="H8:H71" si="1">(E8-D8)*24</f>
-        <v>0.31666666666666821</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="33"/>
-      <c r="B9" s="14">
-        <v>6977</v>
-      </c>
-      <c r="C9" s="22">
-        <v>43930</v>
-      </c>
-      <c r="D9" s="20">
-        <v>0.95833333333333337</v>
-      </c>
-      <c r="E9" s="23">
-        <v>0.96388888888888891</v>
-      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="23"/>
       <c r="F9" s="34"/>
-      <c r="G9" s="17" t="s">
-        <v>19</v>
-      </c>
+      <c r="G9" s="17"/>
       <c r="H9" s="27">
         <f t="shared" si="1"/>
-        <v>0.13333333333333286</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="33"/>
-      <c r="B10" s="14">
-        <v>6977</v>
-      </c>
-      <c r="C10" s="22">
-        <v>43930</v>
-      </c>
-      <c r="D10" s="20">
-        <v>0.96388888888888891</v>
-      </c>
-      <c r="E10" s="23">
-        <v>0.97152777777777777</v>
-      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="23"/>
       <c r="F10" s="34"/>
-      <c r="G10" s="17" t="s">
-        <v>20</v>
-      </c>
+      <c r="G10" s="17"/>
       <c r="H10" s="27">
         <f t="shared" si="1"/>
-        <v>0.18333333333333268</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="33"/>
-      <c r="B11" s="14">
-        <v>6977</v>
-      </c>
-      <c r="C11" s="22">
-        <v>43930</v>
-      </c>
-      <c r="D11" s="20">
-        <v>0.97152777777777777</v>
-      </c>
-      <c r="E11" s="23">
-        <v>0.9770833333333333</v>
-      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="23"/>
       <c r="F11" s="34"/>
-      <c r="G11" s="17" t="s">
-        <v>21</v>
-      </c>
+      <c r="G11" s="17"/>
       <c r="H11" s="27">
         <f t="shared" si="1"/>
-        <v>0.13333333333333286</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="33"/>
-      <c r="B12" s="14">
-        <v>6977</v>
-      </c>
-      <c r="C12" s="22">
-        <v>43931</v>
-      </c>
-      <c r="D12" s="20">
-        <v>2.7083333333333334E-2</v>
-      </c>
-      <c r="E12" s="23">
-        <v>7.2916666666666671E-2</v>
-      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="23"/>
       <c r="F12" s="34"/>
-      <c r="G12" s="17" t="s">
-        <v>37</v>
-      </c>
+      <c r="G12" s="17"/>
       <c r="H12" s="27">
         <f t="shared" si="1"/>
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="33"/>
-      <c r="B13" s="14">
-        <v>6977</v>
-      </c>
-      <c r="C13" s="22">
-        <v>43931</v>
-      </c>
-      <c r="D13" s="20">
-        <v>7.2916666666666671E-2</v>
-      </c>
-      <c r="E13" s="23">
-        <v>0.15625</v>
-      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="23"/>
       <c r="F13" s="34"/>
-      <c r="G13" s="17" t="s">
-        <v>22</v>
-      </c>
+      <c r="G13" s="17"/>
       <c r="H13" s="27">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="33"/>
-      <c r="B14" s="14">
-        <v>6977</v>
-      </c>
-      <c r="C14" s="22">
-        <v>43931</v>
-      </c>
-      <c r="D14" s="20">
-        <v>0.15625</v>
-      </c>
-      <c r="E14" s="23">
-        <v>0.17361111111111113</v>
-      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="23"/>
       <c r="F14" s="34"/>
-      <c r="G14" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="G14" s="17"/>
       <c r="H14" s="27">
         <f t="shared" si="1"/>
-        <v>0.41666666666666718</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="33"/>
-      <c r="B15" s="14">
-        <v>6977</v>
-      </c>
-      <c r="C15" s="22">
-        <v>43931</v>
-      </c>
-      <c r="D15" s="20">
-        <v>0.17361111111111113</v>
-      </c>
-      <c r="E15" s="23">
-        <v>0.19791666666666666</v>
-      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="23"/>
       <c r="F15" s="34"/>
-      <c r="G15" s="17" t="s">
-        <v>24</v>
-      </c>
+      <c r="G15" s="17"/>
       <c r="H15" s="27">
         <f t="shared" si="1"/>
-        <v>0.58333333333333259</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="33"/>
-      <c r="B16" s="14">
-        <v>6977</v>
-      </c>
-      <c r="C16" s="22">
-        <v>43931</v>
-      </c>
-      <c r="D16" s="20">
-        <v>0.19791666666666666</v>
-      </c>
-      <c r="E16" s="23">
-        <v>0.22916666666666666</v>
-      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="23"/>
       <c r="F16" s="34"/>
-      <c r="G16" s="17" t="s">
-        <v>25</v>
-      </c>
+      <c r="G16" s="17"/>
       <c r="H16" s="27">
         <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="33"/>
-      <c r="B17" s="14">
-        <v>6977</v>
-      </c>
-      <c r="C17" s="22">
-        <v>43931</v>
-      </c>
-      <c r="D17" s="20">
-        <v>0.89583333333333337</v>
-      </c>
-      <c r="E17" s="23">
-        <v>0.90625</v>
-      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="23"/>
       <c r="F17" s="34"/>
-      <c r="G17" s="17" t="s">
-        <v>26</v>
-      </c>
+      <c r="G17" s="17"/>
       <c r="H17" s="27">
         <f t="shared" si="1"/>
-        <v>0.24999999999999911</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="33"/>
-      <c r="B18" s="14">
-        <v>6977</v>
-      </c>
-      <c r="C18" s="22">
-        <v>43931</v>
-      </c>
-      <c r="D18" s="20">
-        <v>0.90625</v>
-      </c>
-      <c r="E18" s="23">
-        <v>0.95833333333333337</v>
-      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="23"/>
       <c r="F18" s="34"/>
-      <c r="G18" s="17" t="s">
-        <v>27</v>
-      </c>
+      <c r="G18" s="17"/>
       <c r="H18" s="27">
         <f t="shared" si="1"/>
-        <v>1.2500000000000009</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="33"/>
-      <c r="B19" s="14">
-        <v>6977</v>
-      </c>
-      <c r="C19" s="22">
-        <v>43932</v>
-      </c>
-      <c r="D19" s="20">
-        <v>0.875</v>
-      </c>
-      <c r="E19" s="23">
-        <v>0.89583333333333337</v>
-      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="23"/>
       <c r="F19" s="34"/>
-      <c r="G19" s="17" t="s">
-        <v>28</v>
-      </c>
+      <c r="G19" s="17"/>
       <c r="H19" s="27">
         <f t="shared" si="1"/>
-        <v>0.50000000000000089</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="33"/>
-      <c r="B20" s="14">
-        <v>6977</v>
-      </c>
-      <c r="C20" s="22">
-        <v>43932</v>
-      </c>
-      <c r="D20" s="20">
-        <v>0.89583333333333337</v>
-      </c>
-      <c r="E20" s="23">
-        <v>0.90972222222222221</v>
-      </c>
+      <c r="B20" s="14"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="23"/>
       <c r="F20" s="34"/>
-      <c r="G20" s="17" t="s">
-        <v>30</v>
-      </c>
+      <c r="G20" s="17"/>
       <c r="H20" s="27">
         <f t="shared" si="1"/>
-        <v>0.33333333333333215</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="33"/>
-      <c r="B21" s="14">
-        <v>6977</v>
-      </c>
-      <c r="C21" s="22">
-        <v>43932</v>
-      </c>
-      <c r="D21" s="20">
-        <v>0.90972222222222221</v>
-      </c>
-      <c r="E21" s="23">
-        <v>0.93402777777777779</v>
-      </c>
+      <c r="B21" s="14"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="23"/>
       <c r="F21" s="34"/>
-      <c r="G21" s="17" t="s">
-        <v>29</v>
-      </c>
+      <c r="G21" s="17"/>
       <c r="H21" s="27">
         <f t="shared" si="1"/>
-        <v>0.58333333333333393</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="33"/>
-      <c r="B22" s="14">
-        <v>6977</v>
-      </c>
-      <c r="C22" s="22">
-        <v>43932</v>
-      </c>
-      <c r="D22" s="20">
-        <v>0.93402777777777779</v>
-      </c>
-      <c r="E22" s="23">
-        <v>0.96875</v>
-      </c>
+      <c r="B22" s="14"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="23"/>
       <c r="F22" s="34"/>
-      <c r="G22" s="17" t="s">
-        <v>31</v>
-      </c>
+      <c r="G22" s="17"/>
       <c r="H22" s="27">
         <f t="shared" si="1"/>
-        <v>0.83333333333333304</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="33"/>
-      <c r="B23" s="14">
-        <v>6977</v>
-      </c>
-      <c r="C23" s="22">
-        <v>43932</v>
-      </c>
-      <c r="D23" s="20">
-        <v>0.96875</v>
-      </c>
-      <c r="E23" s="23">
-        <v>0.99930555555555556</v>
-      </c>
+      <c r="B23" s="14"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="23"/>
       <c r="F23" s="34"/>
-      <c r="G23" s="17" t="s">
-        <v>32</v>
-      </c>
+      <c r="G23" s="17"/>
       <c r="H23" s="27">
         <f t="shared" si="1"/>
-        <v>0.73333333333333339</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="33"/>
-      <c r="B24" s="14">
-        <v>6977</v>
-      </c>
-      <c r="C24" s="22">
-        <v>43933</v>
-      </c>
-      <c r="D24" s="20">
-        <v>0.69791666666666663</v>
-      </c>
-      <c r="E24" s="23">
-        <v>0.73958333333333337</v>
-      </c>
+      <c r="B24" s="14"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="23"/>
       <c r="F24" s="34"/>
-      <c r="G24" s="17" t="s">
-        <v>33</v>
-      </c>
+      <c r="G24" s="17"/>
       <c r="H24" s="27">
         <f t="shared" si="1"/>
-        <v>1.0000000000000018</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="33"/>
-      <c r="B25" s="14">
-        <v>6977</v>
-      </c>
-      <c r="C25" s="22">
-        <v>43933</v>
-      </c>
-      <c r="D25" s="20">
-        <v>0.73958333333333337</v>
-      </c>
-      <c r="E25" s="23">
-        <v>0.80208333333333337</v>
-      </c>
+      <c r="B25" s="14"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="23"/>
       <c r="F25" s="34"/>
-      <c r="G25" s="17" t="s">
-        <v>34</v>
-      </c>
+      <c r="G25" s="17"/>
       <c r="H25" s="27">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="33"/>
-      <c r="B26" s="14">
-        <v>6977</v>
-      </c>
-      <c r="C26" s="22">
-        <v>43933</v>
-      </c>
-      <c r="D26" s="20">
-        <v>0.80208333333333337</v>
-      </c>
-      <c r="E26" s="23">
-        <v>0.83333333333333337</v>
-      </c>
+      <c r="B26" s="14"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="23"/>
       <c r="F26" s="34"/>
-      <c r="G26" s="17" t="s">
-        <v>35</v>
-      </c>
+      <c r="G26" s="17"/>
       <c r="H26" s="27">
         <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="33"/>
-      <c r="B27" s="14">
-        <v>6977</v>
-      </c>
-      <c r="C27" s="22">
-        <v>43933</v>
-      </c>
-      <c r="D27" s="20">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="E27" s="23">
-        <v>0.84444444444444444</v>
-      </c>
+      <c r="B27" s="14"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="23"/>
       <c r="F27" s="34"/>
-      <c r="G27" s="17" t="s">
-        <v>36</v>
-      </c>
+      <c r="G27" s="17"/>
       <c r="H27" s="27">
         <f t="shared" si="1"/>
-        <v>0.26666666666666572</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="33"/>
-      <c r="B28" s="14">
-        <v>6977</v>
-      </c>
-      <c r="C28" s="22">
-        <v>43933</v>
-      </c>
-      <c r="D28" s="20">
-        <v>0.84444444444444444</v>
-      </c>
-      <c r="E28" s="23">
-        <v>0.84583333333333333</v>
-      </c>
+      <c r="B28" s="14"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="23"/>
       <c r="F28" s="34"/>
-      <c r="G28" s="17" t="s">
-        <v>38</v>
-      </c>
+      <c r="G28" s="17"/>
       <c r="H28" s="27">
         <f t="shared" si="1"/>
-        <v>3.3333333333333215E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="33"/>
-      <c r="B29" s="14">
-        <v>6977</v>
-      </c>
-      <c r="C29" s="22">
-        <v>43933</v>
-      </c>
-      <c r="D29" s="20">
-        <v>0.84583333333333333</v>
-      </c>
-      <c r="E29" s="23">
-        <v>0.85069444444444453</v>
-      </c>
+      <c r="B29" s="14"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="23"/>
       <c r="F29" s="34"/>
-      <c r="G29" s="17" t="s">
-        <v>39</v>
-      </c>
+      <c r="G29" s="17"/>
       <c r="H29" s="27">
         <f t="shared" si="1"/>
-        <v>0.11666666666666892</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="33"/>
-      <c r="B30" s="14">
-        <v>6977</v>
-      </c>
-      <c r="C30" s="22">
-        <v>43933</v>
-      </c>
-      <c r="D30" s="20">
-        <v>0.85069444444444453</v>
-      </c>
-      <c r="E30" s="23">
-        <v>0.85763888888888884</v>
-      </c>
+      <c r="B30" s="14"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="23"/>
       <c r="F30" s="34"/>
-      <c r="G30" s="17" t="s">
-        <v>40</v>
-      </c>
+      <c r="G30" s="17"/>
       <c r="H30" s="27">
         <f t="shared" si="1"/>
-        <v>0.16666666666666341</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="33"/>
-      <c r="B31" s="14">
-        <v>6977</v>
-      </c>
-      <c r="C31" s="22">
-        <v>43933</v>
-      </c>
-      <c r="D31" s="20">
-        <v>0.85763888888888884</v>
-      </c>
-      <c r="E31" s="23">
-        <v>0.86111111111111116</v>
-      </c>
+      <c r="B31" s="14"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="23"/>
       <c r="F31" s="34"/>
-      <c r="G31" s="17" t="s">
-        <v>41</v>
-      </c>
+      <c r="G31" s="17"/>
       <c r="H31" s="27">
         <f t="shared" si="1"/>
-        <v>8.3333333333335702E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5831,7 +6103,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>14.616666666666671</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6546,7 +6818,7 @@
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="H6:H78">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added in part 1 logs into log file
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0ECF5C-F8EF-4D7E-8524-486E616B6C1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B145391-FFBE-41B7-95C8-29DCAD8C45F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="130">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -204,12 +204,6 @@
     <t>Read notes on how to build a proper barrel shifter for shifting logical and shifting right arithmetic. Got very tired and decided to work on this tomorrow. Updated team members on progress. -NOT DONE</t>
   </si>
   <si>
-    <t>Fixed obvious compilation errors on ModelSim as best as possbile. Rest of compilation errors will be dealt with tomorrow. Pushed changes before going to sleep. -NOT DONE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fixed </t>
-  </si>
-  <si>
     <t>Added placeholder code into barrel shifter .vhd files to compile project on ModelSim. -DONE</t>
   </si>
   <si>
@@ -255,16 +249,229 @@
     <t>Asked team members on progress to be briefed on what needs to be done so that I can work on it when I am available. -DONE</t>
   </si>
   <si>
-    <t>Fixed Part 2 logs as per feedback from part 1. -DONE</t>
-  </si>
-  <si>
     <t>Added incontent from part 1 into Google Doc file. Returned back to other assignments - DONE</t>
   </si>
   <si>
     <t>Read feedback comments from part 1. -DONE</t>
   </si>
   <si>
-    <t>Pulled changes from Github to go over changes team members have made in the past few days. -DONE</t>
+    <t>Pulled changes from Github. Verifying changes team members have made to .vhd files in the past few days. -DONE</t>
+  </si>
+  <si>
+    <t>Compiled all project files on ModelSim and Quartus to verify it compiles. -DONE</t>
+  </si>
+  <si>
+    <t>Verified that all synthesised circuits are correct and looks good. -DONE</t>
+  </si>
+  <si>
+    <t>Verified that all timing simulations are correct and looks good. -DONE</t>
+  </si>
+  <si>
+    <t>Verfied that all functional simulations are correct and looks good. -DONE</t>
+  </si>
+  <si>
+    <t>Rewrite SLL64.vhd, SRA64.vhd and SRL64.vhd for better readiability. -DONE</t>
+  </si>
+  <si>
+    <t>Added documentation on VHDL interface for barrel shifters into Google Doc. -DONE</t>
+  </si>
+  <si>
+    <t>Fixed obvious compilation errors. Rest of compilation errors will be dealt with tomorrow. Pushed changes before going to sleep. -NOT DONE</t>
+  </si>
+  <si>
+    <t>Fixed Part 2 logs as per feedback from part 1. Added in Part 1 into the same log file. -DONE</t>
+  </si>
+  <si>
+    <t>Downloaded and unzipped the project file. Uploaded files into GitHub</t>
+  </si>
+  <si>
+    <t>Organised and moved project files into the "tree of folders" as specified in Page 3 of Instructions. DONE</t>
+  </si>
+  <si>
+    <t>Wrote first few entries into activity log. Created a draft of "FPI-Report-G47-350-1202.docx"</t>
+  </si>
+  <si>
+    <t>Mild symptoms. Will rest and continue work on it next week</t>
+  </si>
+  <si>
+    <t>Updated files from 1.1 to 1.4</t>
+  </si>
+  <si>
+    <t>Updated Final Project PDF document with own name and student number.</t>
+  </si>
+  <si>
+    <t>Updated folders as per instructions. Set up ModelSim and Quartus project files</t>
+  </si>
+  <si>
+    <t>Created a draft of LogicUnit.vhd (have not compiled it yet)</t>
+  </si>
+  <si>
+    <t>Copied over Lab 2 into Adder.vhd (have not compiled it yet)</t>
+  </si>
+  <si>
+    <t>Formatted LogicUnit.vhd and Adder.vhd to look nicer</t>
+  </si>
+  <si>
+    <t>Started work on ArithUnit.vhd. Stopped to look back at notes to fully understand Arithmetic Unit before continueing</t>
+  </si>
+  <si>
+    <t>Fixing LogicUnit.vhd, Adder.vhd and ArithUnit.vhd to make it compile Quartus. Not done</t>
+  </si>
+  <si>
+    <t>Updated .gitignore to ignore some of the Quartus generated files</t>
+  </si>
+  <si>
+    <t>Updated .gitignore to ignore Office temporary files. Makes it annoying to accidentally include temporary files to commit</t>
+  </si>
+  <si>
+    <t>Updated .gitignore to ignore ModelSim and more Quartus generated files</t>
+  </si>
+  <si>
+    <t>Created LogicGates.vhd to include logic gates for the LogicUnit.vhd. Fixed compilation issues with LogicGates.vhd.</t>
+  </si>
+  <si>
+    <t>Fixed possible compilation issue with Adder.vhd (untested)</t>
+  </si>
+  <si>
+    <t>Compiled LogicUnit.vhd successfully. Renamed files according to PDF document and moved them into Documentation folder</t>
+  </si>
+  <si>
+    <t>Fixed folder structure and files as they were incorrect. Fixed project file settings</t>
+  </si>
+  <si>
+    <t>Ran scripts for Test Benches and ConfigExU. Fixed changes along the way (but still does not run successfully)</t>
+  </si>
+  <si>
+    <t>Fixed ArithUnit.vhd and Adder.vhd so they compile on ModelSim and Quartus. DONE</t>
+  </si>
+  <si>
+    <t>Fixed ArithUnit.vhd and Adder.vhd such that both .do scripts work (previosuly they do not work as pointed out by my teammates). Each script works if and only if all ports are defined properly. DONE</t>
+  </si>
+  <si>
+    <t>Generated the functional waveforms of the LogicUnit.vhd. Exported them into Documentation as per instructions</t>
+  </si>
+  <si>
+    <t>Systhesied circuits. Will grab the images later.</t>
+  </si>
+  <si>
+    <t>Set up files and environment to obtain timing simulations from ModelSim. DONE</t>
+  </si>
+  <si>
+    <t>Updated .gitignore to ignore transcript files</t>
+  </si>
+  <si>
+    <t>Obtained timing waveforms and added them to Documentation as per instructions. DONE</t>
+  </si>
+  <si>
+    <t>Added TestVectors. Discovered a bug in LogicUnit.vhd before stopping for dinner.</t>
+  </si>
+  <si>
+    <t>Fixed LogicUnit.vhd.</t>
+  </si>
+  <si>
+    <t>Updated Functional Waveforms for LogicUnit.vhd. DONE</t>
+  </si>
+  <si>
+    <t>Created RTL netlist images and Post-fit images. DONE</t>
+  </si>
+  <si>
+    <t>Updated Timing waveforms for LogicUnit.vhd. DONE</t>
+  </si>
+  <si>
+    <t>Updated folder structure of Documentation directory. Started working on the report.</t>
+  </si>
+  <si>
+    <t>Added overview sections of LogicUnit to report. Noticed that Truth table documented is different than VHDL code</t>
+  </si>
+  <si>
+    <t>Re-compiled VHDL code for LogicUnit.vhd. DONE</t>
+  </si>
+  <si>
+    <t>Renamed .vho and .sdo files for LogicUnit. Exported .vho, .sdo, .map.summary and .fit.summary files to Documentation folder of LogicUnit. DONE</t>
+  </si>
+  <si>
+    <t>Added waveforms for LogicUnit.vhd to document</t>
+  </si>
+  <si>
+    <t>Helped teammates debug VHDL implementation for ArithUnit.vhd and Adder.vhd.</t>
+  </si>
+  <si>
+    <t>Begin annotation of waveform diagrams for LogicUnit.vhd</t>
+  </si>
+  <si>
+    <t>Updated document. Added annotated waveform diagrams to document. Will continue work on document tomorrow</t>
+  </si>
+  <si>
+    <t>Provided tech support to give team members access to Github repository</t>
+  </si>
+  <si>
+    <t>Reviewing team mates' work on Arith.vhd, Adder.vhd and related files. Discovered things that need to be changed.</t>
+  </si>
+  <si>
+    <t>Fixed formatting of Arith.vhd and Adder.vhd. Removed unnecessary comments. DONE</t>
+  </si>
+  <si>
+    <t>Removed unnecessary VHDL code from LogicUnit.vhd. DONE</t>
+  </si>
+  <si>
+    <t>Validated and verified waveforms for ArithUnit.vhd and Adder.vhd. DONE</t>
+  </si>
+  <si>
+    <t>Re-compiled VHDL code for LogicUnit.vhd, Adder.vhd and ArithUnit.vhd. DONE</t>
+  </si>
+  <si>
+    <t>Updated all summary files, .vho files and .sdo files. DONE</t>
+  </si>
+  <si>
+    <t>Removed .gitignore rule for transcript files.</t>
+  </si>
+  <si>
+    <t>Consolidated all files except for report document into one folder to get ready for submission.</t>
+  </si>
+  <si>
+    <t>Re-formatted and edited own log file to make it tidier.</t>
+  </si>
+  <si>
+    <t>After pulling changes form team members, consolidated more files (including report) into folder.</t>
+  </si>
+  <si>
+    <t>Reviewing team mates' work on report. Updating report document (content and formatting). NOT DONE</t>
+  </si>
+  <si>
+    <t>Discovered bug in LogicGate.vhd that does not allow it to compile on ModelSim. Fixed it together with teammates.</t>
+  </si>
+  <si>
+    <t>Verified project download works on a fresh installation of the project. Teammates had discovered this issue earlier and is a source of a massive headache.</t>
+  </si>
+  <si>
+    <t>Re-compiled all VHD files and checked that all results are the same. Updated transcript , summary, .vho and .sdo files. DONE</t>
+  </si>
+  <si>
+    <t>Updated document report. Updated cover page. Fixed formatting. NOT DONE</t>
+  </si>
+  <si>
+    <t>Renamed "FPI-Report-G47-350-1202.docx" to "FPI-Report-G47-350-1201.docx". Passed the document to team mates to work on other stuff due tonight.</t>
+  </si>
+  <si>
+    <t>Assist with writing the report with bits and pieces, here and there.</t>
+  </si>
+  <si>
+    <t>Submitted first attempt to Canvas. Just in case</t>
+  </si>
+  <si>
+    <t>Reviewed report. Fixed spelling, formatting and grammer issues. DONE</t>
+  </si>
+  <si>
+    <t>Submitted second attempt to Canvas. DONE</t>
+  </si>
+  <si>
+    <t>Reviewed report together with team member for possible issues.</t>
+  </si>
+  <si>
+    <t>Revised report together with team member for clarity</t>
+  </si>
+  <si>
+    <t>Last attempt of submission to Canvas. DONE</t>
   </si>
 </sst>
 </file>
@@ -1070,8 +1277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090E6E40-83BD-4CBB-97D3-102021CD8368}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G65" sqref="A65:G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,52 +1364,92 @@
     </row>
     <row r="6" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21"/>
+      <c r="B6" s="13">
+        <v>6977</v>
+      </c>
+      <c r="C6" s="19">
+        <v>43916</v>
+      </c>
+      <c r="D6" s="20">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="E6" s="21">
+        <v>0.9</v>
+      </c>
       <c r="F6" s="32"/>
-      <c r="G6" s="16"/>
+      <c r="G6" s="16" t="s">
+        <v>66</v>
+      </c>
       <c r="H6" s="12">
         <f t="shared" ref="H6" si="0">(E6-D6)*24</f>
-        <v>0</v>
+        <v>9.9999999999999645E-2</v>
       </c>
       <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="23"/>
+      <c r="B7" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C7" s="22">
+        <v>43916</v>
+      </c>
+      <c r="D7" s="20">
+        <v>0.9</v>
+      </c>
+      <c r="E7" s="23">
+        <v>0.91111111111111109</v>
+      </c>
       <c r="F7" s="34"/>
-      <c r="G7" s="17"/>
+      <c r="G7" s="17" t="s">
+        <v>67</v>
+      </c>
       <c r="H7" s="27">
         <f>(E7-D7)*24</f>
-        <v>0</v>
+        <v>0.26666666666666572</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="33"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="23"/>
+      <c r="B8" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C8" s="22">
+        <v>43916</v>
+      </c>
+      <c r="D8" s="20">
+        <v>0.91111111111111109</v>
+      </c>
+      <c r="E8" s="23">
+        <v>0.91319444444444453</v>
+      </c>
       <c r="F8" s="34"/>
-      <c r="G8" s="17"/>
+      <c r="G8" s="17" t="s">
+        <v>68</v>
+      </c>
       <c r="H8" s="27">
         <f t="shared" ref="H8:H71" si="1">(E8-D8)*24</f>
-        <v>0</v>
+        <v>5.0000000000002487E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="33"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="23"/>
+      <c r="B9" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C9" s="22">
+        <v>43918</v>
+      </c>
+      <c r="D9" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="23">
+        <v>0.5</v>
+      </c>
       <c r="F9" s="34"/>
-      <c r="G9" s="17"/>
+      <c r="G9" s="17" t="s">
+        <v>69</v>
+      </c>
       <c r="H9" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1210,821 +1457,1451 @@
     </row>
     <row r="10" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="33"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="23"/>
+      <c r="B10" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C10" s="22">
+        <v>43923</v>
+      </c>
+      <c r="D10" s="20">
+        <v>0.83888888888888891</v>
+      </c>
+      <c r="E10" s="23">
+        <v>0.84166666666666667</v>
+      </c>
       <c r="F10" s="34"/>
-      <c r="G10" s="17"/>
+      <c r="G10" s="17" t="s">
+        <v>70</v>
+      </c>
       <c r="H10" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.666666666666643E-2</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="33"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="23"/>
+      <c r="B11" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C11" s="22">
+        <v>43923</v>
+      </c>
+      <c r="D11" s="20">
+        <v>0.3430555555555555</v>
+      </c>
+      <c r="E11" s="23">
+        <v>0.3444444444444445</v>
+      </c>
       <c r="F11" s="34"/>
-      <c r="G11" s="17"/>
+      <c r="G11" s="17" t="s">
+        <v>71</v>
+      </c>
       <c r="H11" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.3333333333335879E-2</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="33"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="23"/>
+      <c r="B12" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C12" s="22">
+        <v>43923</v>
+      </c>
+      <c r="D12" s="20">
+        <v>0.8833333333333333</v>
+      </c>
+      <c r="E12" s="23">
+        <v>0.9243055555555556</v>
+      </c>
       <c r="F12" s="34"/>
-      <c r="G12" s="17"/>
+      <c r="G12" s="17" t="s">
+        <v>72</v>
+      </c>
       <c r="H12" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.98333333333333517</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="33"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="23"/>
+      <c r="B13" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C13" s="22">
+        <v>43923</v>
+      </c>
+      <c r="D13" s="20">
+        <v>0.96875</v>
+      </c>
+      <c r="E13" s="23">
+        <v>0.99930555555555556</v>
+      </c>
       <c r="F13" s="34"/>
-      <c r="G13" s="17"/>
+      <c r="G13" s="17" t="s">
+        <v>73</v>
+      </c>
       <c r="H13" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.73333333333333339</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="33"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="23"/>
+      <c r="B14" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C14" s="22">
+        <v>43924</v>
+      </c>
+      <c r="D14" s="20">
+        <v>0</v>
+      </c>
+      <c r="E14" s="23">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="F14" s="34"/>
-      <c r="G14" s="17"/>
+      <c r="G14" s="17" t="s">
+        <v>74</v>
+      </c>
       <c r="H14" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="33"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="23"/>
+      <c r="B15" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C15" s="22">
+        <v>43924</v>
+      </c>
+      <c r="D15" s="20">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E15" s="23">
+        <v>3.125E-2</v>
+      </c>
       <c r="F15" s="34"/>
-      <c r="G15" s="17"/>
+      <c r="G15" s="17" t="s">
+        <v>75</v>
+      </c>
       <c r="H15" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="33"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="23"/>
+      <c r="B16" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C16" s="22">
+        <v>43924</v>
+      </c>
+      <c r="D16" s="20">
+        <v>3.8194444444444441E-2</v>
+      </c>
+      <c r="E16" s="23">
+        <v>5.5555555555555552E-2</v>
+      </c>
       <c r="F16" s="34"/>
-      <c r="G16" s="17"/>
+      <c r="G16" s="17" t="s">
+        <v>76</v>
+      </c>
       <c r="H16" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="33"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="23"/>
+      <c r="B17" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C17" s="22">
+        <v>43924</v>
+      </c>
+      <c r="D17" s="20">
+        <v>8.4027777777777771E-2</v>
+      </c>
+      <c r="E17" s="23">
+        <v>0.11597222222222221</v>
+      </c>
       <c r="F17" s="34"/>
-      <c r="G17" s="17"/>
+      <c r="G17" s="17" t="s">
+        <v>77</v>
+      </c>
       <c r="H17" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.76666666666666661</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="33"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="23"/>
+      <c r="B18" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C18" s="22">
+        <v>43924</v>
+      </c>
+      <c r="D18" s="20">
+        <v>0.11597222222222221</v>
+      </c>
+      <c r="E18" s="23">
+        <v>0.14166666666666666</v>
+      </c>
       <c r="F18" s="34"/>
-      <c r="G18" s="17"/>
+      <c r="G18" s="17" t="s">
+        <v>78</v>
+      </c>
       <c r="H18" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.61666666666666681</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="33"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="23"/>
+      <c r="B19" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C19" s="22">
+        <v>43924</v>
+      </c>
+      <c r="D19" s="20">
+        <v>0.14166666666666666</v>
+      </c>
+      <c r="E19" s="23">
+        <v>0.14791666666666667</v>
+      </c>
       <c r="F19" s="34"/>
-      <c r="G19" s="17"/>
+      <c r="G19" s="17" t="s">
+        <v>79</v>
+      </c>
       <c r="H19" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.15000000000000013</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="33"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="23"/>
+      <c r="B20" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C20" s="22">
+        <v>43924</v>
+      </c>
+      <c r="D20" s="20">
+        <v>0.83680555555555547</v>
+      </c>
+      <c r="E20" s="23">
+        <v>0.84652777777777777</v>
+      </c>
       <c r="F20" s="34"/>
-      <c r="G20" s="17"/>
+      <c r="G20" s="17" t="s">
+        <v>80</v>
+      </c>
       <c r="H20" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.23333333333333517</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="33"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="23"/>
+      <c r="B21" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C21" s="22">
+        <v>43924</v>
+      </c>
+      <c r="D21" s="20">
+        <v>0.85486111111111107</v>
+      </c>
+      <c r="E21" s="23">
+        <v>0.87222222222222223</v>
+      </c>
       <c r="F21" s="34"/>
-      <c r="G21" s="17"/>
+      <c r="G21" s="17" t="s">
+        <v>81</v>
+      </c>
       <c r="H21" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.41666666666666785</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="33"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="23"/>
+      <c r="B22" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C22" s="22">
+        <v>43924</v>
+      </c>
+      <c r="D22" s="20">
+        <v>0.87222222222222223</v>
+      </c>
+      <c r="E22" s="23">
+        <v>0.87638888888888899</v>
+      </c>
       <c r="F22" s="34"/>
-      <c r="G22" s="17"/>
+      <c r="G22" s="17" t="s">
+        <v>82</v>
+      </c>
       <c r="H22" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.10000000000000231</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="33"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="23"/>
+      <c r="B23" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C23" s="22">
+        <v>43924</v>
+      </c>
+      <c r="D23" s="20">
+        <v>0.87638888888888899</v>
+      </c>
+      <c r="E23" s="23">
+        <v>0.88611111111111107</v>
+      </c>
       <c r="F23" s="34"/>
-      <c r="G23" s="17"/>
+      <c r="G23" s="17" t="s">
+        <v>83</v>
+      </c>
       <c r="H23" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.23333333333332984</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="33"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="23"/>
+      <c r="B24" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C24" s="22">
+        <v>43924</v>
+      </c>
+      <c r="D24" s="20">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="E24" s="23">
+        <v>0.89930555555555547</v>
+      </c>
       <c r="F24" s="34"/>
-      <c r="G24" s="17"/>
+      <c r="G24" s="17" t="s">
+        <v>84</v>
+      </c>
       <c r="H24" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.31666666666666554</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="33"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="23"/>
+      <c r="B25" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C25" s="22">
+        <v>43924</v>
+      </c>
+      <c r="D25" s="20">
+        <v>0.89930555555555547</v>
+      </c>
+      <c r="E25" s="23">
+        <v>0.91319444444444453</v>
+      </c>
       <c r="F25" s="34"/>
-      <c r="G25" s="17"/>
+      <c r="G25" s="17" t="s">
+        <v>85</v>
+      </c>
       <c r="H25" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333748</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="33"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="23"/>
+      <c r="B26" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C26" s="22">
+        <v>43924</v>
+      </c>
+      <c r="D26" s="20">
+        <v>0.91319444444444453</v>
+      </c>
+      <c r="E26" s="23">
+        <v>0.92708333333333337</v>
+      </c>
       <c r="F26" s="34"/>
-      <c r="G26" s="17"/>
+      <c r="G26" s="17" t="s">
+        <v>86</v>
+      </c>
       <c r="H26" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333215</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="33"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="23"/>
+      <c r="B27" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C27" s="22">
+        <v>43924</v>
+      </c>
+      <c r="D27" s="20">
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="E27" s="23">
+        <v>0.96875</v>
+      </c>
       <c r="F27" s="34"/>
-      <c r="G27" s="17"/>
+      <c r="G27" s="17" t="s">
+        <v>87</v>
+      </c>
       <c r="H27" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.99999999999999911</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="33"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="23"/>
+      <c r="B28" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C28" s="22">
+        <v>43924</v>
+      </c>
+      <c r="D28" s="20">
+        <v>0.96875</v>
+      </c>
+      <c r="E28" s="23">
+        <v>0.98958333333333337</v>
+      </c>
       <c r="F28" s="34"/>
-      <c r="G28" s="17"/>
+      <c r="G28" s="17" t="s">
+        <v>88</v>
+      </c>
       <c r="H28" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.50000000000000089</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="33"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="23"/>
+      <c r="B29" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C29" s="22">
+        <v>43924</v>
+      </c>
+      <c r="D29" s="20">
+        <v>0.98958333333333337</v>
+      </c>
+      <c r="E29" s="23">
+        <v>0.99652777777777779</v>
+      </c>
       <c r="F29" s="34"/>
-      <c r="G29" s="17"/>
+      <c r="G29" s="17" t="s">
+        <v>89</v>
+      </c>
       <c r="H29" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.16666666666666607</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="33"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="23"/>
+      <c r="B30" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C30" s="22">
+        <v>43924</v>
+      </c>
+      <c r="D30" s="20">
+        <v>0.99652777777777779</v>
+      </c>
+      <c r="E30" s="23">
+        <v>0.99930555555555556</v>
+      </c>
       <c r="F30" s="34"/>
-      <c r="G30" s="17"/>
+      <c r="G30" s="17" t="s">
+        <v>90</v>
+      </c>
       <c r="H30" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.666666666666643E-2</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="33"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="23"/>
+      <c r="B31" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C31" s="22">
+        <v>43925</v>
+      </c>
+      <c r="D31" s="20">
+        <v>0</v>
+      </c>
+      <c r="E31" s="23">
+        <v>4.8611111111111112E-3</v>
+      </c>
       <c r="F31" s="34"/>
-      <c r="G31" s="17"/>
+      <c r="G31" s="17" t="s">
+        <v>91</v>
+      </c>
       <c r="H31" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.11666666666666667</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="33"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="23"/>
+      <c r="B32" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C32" s="22">
+        <v>43925</v>
+      </c>
+      <c r="D32" s="20">
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="E32" s="23">
+        <v>1.5972222222222224E-2</v>
+      </c>
       <c r="F32" s="34"/>
-      <c r="G32" s="17"/>
+      <c r="G32" s="17" t="s">
+        <v>92</v>
+      </c>
       <c r="H32" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1833333333333334</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="33"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="23"/>
+      <c r="B33" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C33" s="22">
+        <v>43925</v>
+      </c>
+      <c r="D33" s="20">
+        <v>0.7090277777777777</v>
+      </c>
+      <c r="E33" s="23">
+        <v>0.75763888888888886</v>
+      </c>
       <c r="F33" s="34"/>
-      <c r="G33" s="17"/>
+      <c r="G33" s="17" t="s">
+        <v>93</v>
+      </c>
       <c r="H33" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.1666666666666679</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="33"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="23"/>
+      <c r="B34" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C34" s="22">
+        <v>43925</v>
+      </c>
+      <c r="D34" s="20">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="E34" s="23">
+        <v>0.92708333333333337</v>
+      </c>
       <c r="F34" s="34"/>
-      <c r="G34" s="17"/>
+      <c r="G34" s="17" t="s">
+        <v>94</v>
+      </c>
       <c r="H34" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.0000000000000018</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="33"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="23"/>
+      <c r="B35" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C35" s="22">
+        <v>43925</v>
+      </c>
+      <c r="D35" s="20">
+        <v>0.93402777777777779</v>
+      </c>
+      <c r="E35" s="23">
+        <v>0.94791666666666663</v>
+      </c>
       <c r="F35" s="34"/>
-      <c r="G35" s="17"/>
+      <c r="G35" s="17" t="s">
+        <v>95</v>
+      </c>
       <c r="H35" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333215</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="33"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="23"/>
+      <c r="B36" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C36" s="22">
+        <v>43925</v>
+      </c>
+      <c r="D36" s="20">
+        <v>0.94791666666666663</v>
+      </c>
+      <c r="E36" s="23">
+        <v>0.96180555555555547</v>
+      </c>
       <c r="F36" s="34"/>
-      <c r="G36" s="17"/>
+      <c r="G36" s="17" t="s">
+        <v>96</v>
+      </c>
       <c r="H36" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333215</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="33"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="23"/>
+      <c r="B37" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C37" s="22">
+        <v>43925</v>
+      </c>
+      <c r="D37" s="20">
+        <v>0.96180555555555547</v>
+      </c>
+      <c r="E37" s="23">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="F37" s="34"/>
-      <c r="G37" s="17"/>
+      <c r="G37" s="17" t="s">
+        <v>97</v>
+      </c>
       <c r="H37" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.41666666666666785</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="33"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="23"/>
+      <c r="B38" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C38" s="22">
+        <v>43925</v>
+      </c>
+      <c r="D38" s="20">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="E38" s="23">
+        <v>0.98749999999999993</v>
+      </c>
       <c r="F38" s="34"/>
-      <c r="G38" s="17"/>
+      <c r="G38" s="17" t="s">
+        <v>98</v>
+      </c>
       <c r="H38" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.19999999999999929</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="33"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="23"/>
+      <c r="B39" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C39" s="22">
+        <v>43925</v>
+      </c>
+      <c r="D39" s="20">
+        <v>0.98749999999999993</v>
+      </c>
+      <c r="E39" s="23">
+        <v>0.99930555555555556</v>
+      </c>
       <c r="F39" s="34"/>
-      <c r="G39" s="17"/>
+      <c r="G39" s="17" t="s">
+        <v>99</v>
+      </c>
       <c r="H39" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.28333333333333499</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="33"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="23"/>
+      <c r="B40" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C40" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D40" s="20">
+        <v>0</v>
+      </c>
+      <c r="E40" s="23">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="F40" s="34"/>
-      <c r="G40" s="17"/>
+      <c r="G40" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="H40" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="33"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="23"/>
+      <c r="B41" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C41" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D41" s="20">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E41" s="23">
+        <v>3.6111111111111115E-2</v>
+      </c>
       <c r="F41" s="34"/>
-      <c r="G41" s="17"/>
+      <c r="G41" s="17" t="s">
+        <v>95</v>
+      </c>
       <c r="H41" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.36666666666666681</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="33"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="23"/>
+      <c r="B42" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C42" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D42" s="20">
+        <v>3.6111111111111115E-2</v>
+      </c>
+      <c r="E42" s="23">
+        <v>5.9722222222222225E-2</v>
+      </c>
       <c r="F42" s="34"/>
-      <c r="G42" s="17"/>
+      <c r="G42" s="17" t="s">
+        <v>101</v>
+      </c>
       <c r="H42" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.56666666666666665</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="33"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="23"/>
+      <c r="B43" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C43" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D43" s="20">
+        <v>5.9722222222222225E-2</v>
+      </c>
+      <c r="E43" s="23">
+        <v>6.8749999999999992E-2</v>
+      </c>
       <c r="F43" s="34"/>
-      <c r="G43" s="17"/>
+      <c r="G43" s="17" t="s">
+        <v>97</v>
+      </c>
       <c r="H43" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.2166666666666664</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="33"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="23"/>
+      <c r="B44" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C44" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D44" s="20">
+        <v>6.8749999999999992E-2</v>
+      </c>
+      <c r="E44" s="23">
+        <v>7.4305555555555555E-2</v>
+      </c>
       <c r="F44" s="34"/>
-      <c r="G44" s="17"/>
+      <c r="G44" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="H44" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.13333333333333353</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="33"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="22"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="23"/>
+      <c r="B45" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C45" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D45" s="20">
+        <v>7.4305555555555555E-2</v>
+      </c>
+      <c r="E45" s="23">
+        <v>9.375E-2</v>
+      </c>
       <c r="F45" s="34"/>
-      <c r="G45" s="17"/>
+      <c r="G45" s="17" t="s">
+        <v>103</v>
+      </c>
       <c r="H45" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.46666666666666667</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="33"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="22"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="23"/>
+      <c r="B46" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C46" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D46" s="20">
+        <v>9.375E-2</v>
+      </c>
+      <c r="E46" s="23">
+        <v>0.13541666666666666</v>
+      </c>
       <c r="F46" s="34"/>
-      <c r="G46" s="17"/>
+      <c r="G46" s="17" t="s">
+        <v>104</v>
+      </c>
       <c r="H46" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.99999999999999978</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="33"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="22"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="23"/>
+      <c r="B47" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C47" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D47" s="20">
+        <v>0.13541666666666666</v>
+      </c>
+      <c r="E47" s="23">
+        <v>0.15625</v>
+      </c>
       <c r="F47" s="34"/>
-      <c r="G47" s="17"/>
+      <c r="G47" s="17" t="s">
+        <v>105</v>
+      </c>
       <c r="H47" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.50000000000000022</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="33"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="22"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="23"/>
+      <c r="B48" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C48" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D48" s="20">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E48" s="23">
+        <v>0.61805555555555558</v>
+      </c>
       <c r="F48" s="34"/>
-      <c r="G48" s="17"/>
+      <c r="G48" s="17" t="s">
+        <v>106</v>
+      </c>
       <c r="H48" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333481</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="33"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="22"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="23"/>
+      <c r="B49" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C49" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D49" s="20">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="E49" s="23">
+        <v>0.63541666666666663</v>
+      </c>
       <c r="F49" s="34"/>
-      <c r="G49" s="17"/>
+      <c r="G49" s="17" t="s">
+        <v>107</v>
+      </c>
       <c r="H49" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.41666666666666519</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="33"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="22"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="23"/>
+      <c r="B50" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C50" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D50" s="20">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="E50" s="23">
+        <v>0.64236111111111105</v>
+      </c>
       <c r="F50" s="34"/>
-      <c r="G50" s="17"/>
+      <c r="G50" s="17" t="s">
+        <v>108</v>
+      </c>
       <c r="H50" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.16666666666666607</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="33"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="22"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="23"/>
+      <c r="B51" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C51" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D51" s="20">
+        <v>0.64236111111111105</v>
+      </c>
+      <c r="E51" s="23">
+        <v>0.64930555555555558</v>
+      </c>
       <c r="F51" s="34"/>
-      <c r="G51" s="17"/>
+      <c r="G51" s="17" t="s">
+        <v>109</v>
+      </c>
       <c r="H51" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.16666666666666874</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="33"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="22"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="23"/>
+      <c r="B52" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C52" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D52" s="20">
+        <v>0.64930555555555558</v>
+      </c>
+      <c r="E52" s="23">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="F52" s="34"/>
-      <c r="G52" s="17"/>
+      <c r="G52" s="17" t="s">
+        <v>110</v>
+      </c>
       <c r="H52" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.416666666666667</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="33"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="22"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="23"/>
+      <c r="B53" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C53" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D53" s="20">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="E53" s="23">
+        <v>0.76041666666666663</v>
+      </c>
       <c r="F53" s="34"/>
-      <c r="G53" s="17"/>
+      <c r="G53" s="17" t="s">
+        <v>111</v>
+      </c>
       <c r="H53" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.49999999999999822</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="33"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="22"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="23"/>
+      <c r="B54" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C54" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D54" s="20">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="E54" s="23">
+        <v>0.77916666666666667</v>
+      </c>
       <c r="F54" s="34"/>
-      <c r="G54" s="17"/>
+      <c r="G54" s="17" t="s">
+        <v>112</v>
+      </c>
       <c r="H54" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.45000000000000107</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="33"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="22"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="23"/>
+      <c r="B55" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C55" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D55" s="20">
+        <v>0.77916666666666667</v>
+      </c>
+      <c r="E55" s="23">
+        <v>0.78611111111111109</v>
+      </c>
       <c r="F55" s="34"/>
-      <c r="G55" s="17"/>
+      <c r="G55" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="H55" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.16666666666666607</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="33"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="22"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="23"/>
+      <c r="B56" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C56" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D56" s="20">
+        <v>0.78611111111111109</v>
+      </c>
+      <c r="E56" s="23">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="F56" s="34"/>
-      <c r="G56" s="17"/>
+      <c r="G56" s="17" t="s">
+        <v>106</v>
+      </c>
       <c r="H56" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.13333333333333286</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="33"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="22"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="23"/>
+      <c r="B57" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C57" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D57" s="20">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E57" s="23">
+        <v>0.79861111111111116</v>
+      </c>
       <c r="F57" s="34"/>
-      <c r="G57" s="17"/>
+      <c r="G57" s="17" t="s">
+        <v>114</v>
+      </c>
       <c r="H57" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.16666666666666874</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="33"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="22"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="23"/>
+      <c r="B58" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C58" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D58" s="20">
+        <v>0.79861111111111116</v>
+      </c>
+      <c r="E58" s="23">
+        <v>0.80833333333333324</v>
+      </c>
       <c r="F58" s="34"/>
-      <c r="G58" s="17"/>
+      <c r="G58" s="17" t="s">
+        <v>115</v>
+      </c>
       <c r="H58" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.23333333333332984</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="33"/>
-      <c r="B59" s="14"/>
-      <c r="C59" s="22"/>
-      <c r="D59" s="20"/>
-      <c r="E59" s="23"/>
+      <c r="B59" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C59" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D59" s="20">
+        <v>0.80833333333333324</v>
+      </c>
+      <c r="E59" s="23">
+        <v>0.81180555555555556</v>
+      </c>
       <c r="F59" s="34"/>
-      <c r="G59" s="17"/>
+      <c r="G59" s="17" t="s">
+        <v>116</v>
+      </c>
       <c r="H59" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.3333333333335702E-2</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="33"/>
-      <c r="B60" s="14"/>
-      <c r="C60" s="22"/>
-      <c r="D60" s="20"/>
-      <c r="E60" s="23"/>
+      <c r="B60" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C60" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D60" s="20">
+        <v>0.81180555555555556</v>
+      </c>
+      <c r="E60" s="23">
+        <v>0.82708333333333339</v>
+      </c>
       <c r="F60" s="34"/>
-      <c r="G60" s="17"/>
+      <c r="G60" s="17" t="s">
+        <v>117</v>
+      </c>
       <c r="H60" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.36666666666666803</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="33"/>
-      <c r="B61" s="14"/>
-      <c r="C61" s="22"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="23"/>
+      <c r="B61" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C61" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D61" s="20">
+        <v>0.82708333333333339</v>
+      </c>
+      <c r="E61" s="23">
+        <v>0.84375</v>
+      </c>
       <c r="F61" s="34"/>
-      <c r="G61" s="17"/>
+      <c r="G61" s="17" t="s">
+        <v>118</v>
+      </c>
       <c r="H61" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.39999999999999858</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="33"/>
-      <c r="B62" s="14"/>
-      <c r="C62" s="22"/>
-      <c r="D62" s="20"/>
-      <c r="E62" s="23"/>
+      <c r="B62" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C62" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D62" s="20">
+        <v>0.84375</v>
+      </c>
+      <c r="E62" s="23">
+        <v>0.86041666666666661</v>
+      </c>
       <c r="F62" s="34"/>
-      <c r="G62" s="17"/>
+      <c r="G62" s="17" t="s">
+        <v>119</v>
+      </c>
       <c r="H62" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.39999999999999858</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="33"/>
-      <c r="B63" s="14"/>
-      <c r="C63" s="22"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="23"/>
+      <c r="B63" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C63" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D63" s="20">
+        <v>0.86041666666666661</v>
+      </c>
+      <c r="E63" s="23">
+        <v>0.88194444444444453</v>
+      </c>
       <c r="F63" s="34"/>
-      <c r="G63" s="17"/>
+      <c r="G63" s="17" t="s">
+        <v>120</v>
+      </c>
       <c r="H63" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.51666666666667016</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="33"/>
-      <c r="B64" s="14"/>
-      <c r="C64" s="22"/>
-      <c r="D64" s="20"/>
-      <c r="E64" s="23"/>
+      <c r="B64" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C64" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D64" s="20">
+        <v>0.90347222222222223</v>
+      </c>
+      <c r="E64" s="23">
+        <v>0.91666666666666663</v>
+      </c>
       <c r="F64" s="34"/>
-      <c r="G64" s="17"/>
+      <c r="G64" s="17" t="s">
+        <v>121</v>
+      </c>
       <c r="H64" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.31666666666666554</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="33"/>
-      <c r="B65" s="14"/>
-      <c r="C65" s="22"/>
-      <c r="D65" s="20"/>
-      <c r="E65" s="23"/>
+      <c r="B65" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C65" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D65" s="20">
+        <v>0.93402777777777779</v>
+      </c>
+      <c r="E65" s="23">
+        <v>0.93611111111111101</v>
+      </c>
       <c r="F65" s="34"/>
-      <c r="G65" s="17"/>
+      <c r="G65" s="17" t="s">
+        <v>122</v>
+      </c>
       <c r="H65" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.9999999999997158E-2</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="33"/>
-      <c r="B66" s="14"/>
-      <c r="C66" s="22"/>
-      <c r="D66" s="20"/>
-      <c r="E66" s="23"/>
+      <c r="B66" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C66" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D66" s="20">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E66" s="23">
+        <v>0.96527777777777779</v>
+      </c>
       <c r="F66" s="34"/>
-      <c r="G66" s="17"/>
+      <c r="G66" s="17" t="s">
+        <v>123</v>
+      </c>
       <c r="H66" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.16666666666666607</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="33"/>
-      <c r="B67" s="14"/>
-      <c r="C67" s="22"/>
-      <c r="D67" s="20"/>
-      <c r="E67" s="23"/>
+      <c r="B67" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C67" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D67" s="20">
+        <v>0.96527777777777779</v>
+      </c>
+      <c r="E67" s="23">
+        <v>0.97152777777777777</v>
+      </c>
       <c r="F67" s="34"/>
-      <c r="G67" s="17"/>
+      <c r="G67" s="17" t="s">
+        <v>124</v>
+      </c>
       <c r="H67" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.14999999999999947</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="33"/>
-      <c r="B68" s="14"/>
-      <c r="C68" s="22"/>
-      <c r="D68" s="20"/>
-      <c r="E68" s="23"/>
+      <c r="B68" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C68" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D68" s="20">
+        <v>0.97152777777777777</v>
+      </c>
+      <c r="E68" s="23">
+        <v>0.98263888888888884</v>
+      </c>
       <c r="F68" s="34"/>
-      <c r="G68" s="17"/>
+      <c r="G68" s="17" t="s">
+        <v>125</v>
+      </c>
       <c r="H68" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.26666666666666572</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="33"/>
-      <c r="B69" s="14"/>
-      <c r="C69" s="22"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="23"/>
+      <c r="B69" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C69" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D69" s="20">
+        <v>0.98263888888888884</v>
+      </c>
+      <c r="E69" s="23">
+        <v>0.98402777777777783</v>
+      </c>
       <c r="F69" s="34"/>
-      <c r="G69" s="17"/>
+      <c r="G69" s="17" t="s">
+        <v>126</v>
+      </c>
       <c r="H69" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.3333333333335879E-2</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="33"/>
-      <c r="B70" s="14"/>
-      <c r="C70" s="22"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="23"/>
+      <c r="B70" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C70" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D70" s="20">
+        <v>0.98402777777777783</v>
+      </c>
+      <c r="E70" s="23">
+        <v>0.99097222222222225</v>
+      </c>
       <c r="F70" s="34"/>
-      <c r="G70" s="17"/>
+      <c r="G70" s="17" t="s">
+        <v>127</v>
+      </c>
       <c r="H70" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.16666666666666607</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="33"/>
-      <c r="B71" s="14"/>
-      <c r="C71" s="22"/>
-      <c r="D71" s="20"/>
-      <c r="E71" s="23"/>
+      <c r="B71" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C71" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D71" s="20">
+        <v>0.99097222222222225</v>
+      </c>
+      <c r="E71" s="23">
+        <v>0.99652777777777779</v>
+      </c>
       <c r="F71" s="34"/>
-      <c r="G71" s="17"/>
+      <c r="G71" s="17" t="s">
+        <v>128</v>
+      </c>
       <c r="H71" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.13333333333333286</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="33"/>
-      <c r="B72" s="14"/>
-      <c r="C72" s="22"/>
-      <c r="D72" s="20"/>
-      <c r="E72" s="23"/>
+      <c r="B72" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C72" s="22">
+        <v>43926</v>
+      </c>
+      <c r="D72" s="20">
+        <v>0.99652777777777779</v>
+      </c>
+      <c r="E72" s="23">
+        <v>0.99930555555555556</v>
+      </c>
       <c r="F72" s="34"/>
-      <c r="G72" s="17"/>
+      <c r="G72" s="17" t="s">
+        <v>129</v>
+      </c>
       <c r="H72" s="27">
         <f t="shared" ref="H72:H78" si="2">(E72-D72)*24</f>
-        <v>0</v>
+        <v>6.666666666666643E-2</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -2109,7 +2986,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>0</v>
+        <v>23.683333333333341</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2837,8 +3714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5014613-EBCB-42CE-9E22-81901AAC5CBA}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3422,7 +4299,7 @@
       </c>
       <c r="F27" s="34"/>
       <c r="G27" s="17" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="H27" s="27">
         <f t="shared" si="0"/>
@@ -3441,15 +4318,15 @@
         <v>0.875</v>
       </c>
       <c r="E28" s="23">
-        <v>0.89583333333333337</v>
+        <v>0.90277777777777779</v>
       </c>
       <c r="F28" s="34"/>
       <c r="G28" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H28" s="27">
         <f t="shared" si="0"/>
-        <v>0.50000000000000089</v>
+        <v>0.66666666666666696</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3460,19 +4337,19 @@
       <c r="C29" s="22">
         <v>43932</v>
       </c>
-      <c r="D29" s="23">
-        <v>0.89583333333333337</v>
+      <c r="D29" s="20">
+        <v>0.90277777777777779</v>
       </c>
       <c r="E29" s="23">
-        <v>0.90972222222222221</v>
+        <v>0.92361111111111116</v>
       </c>
       <c r="F29" s="34"/>
       <c r="G29" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H29" s="27">
         <f t="shared" si="0"/>
-        <v>0.33333333333333215</v>
+        <v>0.50000000000000089</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3484,18 +4361,18 @@
         <v>43932</v>
       </c>
       <c r="D30" s="20">
-        <v>0.90972222222222221</v>
+        <v>0.92361111111111116</v>
       </c>
       <c r="E30" s="23">
-        <v>0.92361111111111116</v>
+        <v>0.9375</v>
       </c>
       <c r="F30" s="34"/>
       <c r="G30" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H30" s="27">
         <f t="shared" si="0"/>
-        <v>0.33333333333333481</v>
+        <v>0.33333333333333215</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3507,10 +4384,10 @@
         <v>43932</v>
       </c>
       <c r="D31" s="20">
-        <v>0.92361111111111116</v>
+        <v>0.9375</v>
       </c>
       <c r="E31" s="23">
-        <v>0.9375</v>
+        <v>0.94097222222222221</v>
       </c>
       <c r="F31" s="34"/>
       <c r="G31" s="17" t="s">
@@ -3518,7 +4395,7 @@
       </c>
       <c r="H31" s="27">
         <f t="shared" si="0"/>
-        <v>0.33333333333333215</v>
+        <v>8.3333333333333037E-2</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3530,18 +4407,18 @@
         <v>43932</v>
       </c>
       <c r="D32" s="20">
-        <v>0.9375</v>
+        <v>0.94097222222222221</v>
       </c>
       <c r="E32" s="23">
-        <v>0.94097222222222221</v>
+        <v>0.96875</v>
       </c>
       <c r="F32" s="34"/>
       <c r="G32" s="17" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="H32" s="27">
         <f t="shared" si="0"/>
-        <v>8.3333333333333037E-2</v>
+        <v>0.66666666666666696</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3553,18 +4430,18 @@
         <v>43932</v>
       </c>
       <c r="D33" s="20">
-        <v>0.94097222222222221</v>
+        <v>0.96875</v>
       </c>
       <c r="E33" s="23">
-        <v>0.96875</v>
+        <v>0.99930555555555556</v>
       </c>
       <c r="F33" s="34"/>
       <c r="G33" s="17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H33" s="27">
         <f t="shared" si="0"/>
-        <v>0.66666666666666696</v>
+        <v>0.73333333333333339</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3573,21 +4450,21 @@
         <v>6977</v>
       </c>
       <c r="C34" s="22">
-        <v>43932</v>
+        <v>43933</v>
       </c>
       <c r="D34" s="20">
-        <v>0.96875</v>
+        <v>0.69791666666666663</v>
       </c>
       <c r="E34" s="23">
-        <v>0.99930555555555556</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="F34" s="34"/>
       <c r="G34" s="17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H34" s="27">
         <f t="shared" si="0"/>
-        <v>0.73333333333333339</v>
+        <v>1.0000000000000018</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3599,18 +4476,18 @@
         <v>43933</v>
       </c>
       <c r="D35" s="20">
-        <v>0.69791666666666663</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="E35" s="23">
-        <v>0.73958333333333337</v>
+        <v>0.76388888888888884</v>
       </c>
       <c r="F35" s="34"/>
       <c r="G35" s="17" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="H35" s="27">
         <f t="shared" si="0"/>
-        <v>1.0000000000000018</v>
+        <v>0.58333333333333126</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3622,18 +4499,18 @@
         <v>43933</v>
       </c>
       <c r="D36" s="20">
-        <v>0.73958333333333337</v>
+        <v>0.76388888888888884</v>
       </c>
       <c r="E36" s="23">
-        <v>0.76388888888888884</v>
+        <v>0.80208333333333337</v>
       </c>
       <c r="F36" s="34"/>
       <c r="G36" s="17" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="H36" s="27">
         <f t="shared" si="0"/>
-        <v>0.58333333333333126</v>
+        <v>0.91666666666666874</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3645,18 +4522,18 @@
         <v>43933</v>
       </c>
       <c r="D37" s="20">
-        <v>0.76388888888888884</v>
+        <v>0.80208333333333337</v>
       </c>
       <c r="E37" s="23">
-        <v>0.80208333333333337</v>
+        <v>0.80902777777777779</v>
       </c>
       <c r="F37" s="34"/>
       <c r="G37" s="17" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="H37" s="27">
         <f t="shared" si="0"/>
-        <v>0.91666666666666874</v>
+        <v>0.16666666666666607</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3668,18 +4545,18 @@
         <v>43933</v>
       </c>
       <c r="D38" s="20">
-        <v>0.80208333333333337</v>
+        <v>0.80902777777777779</v>
       </c>
       <c r="E38" s="23">
-        <v>0.80902777777777779</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="F38" s="34"/>
       <c r="G38" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H38" s="27">
         <f t="shared" si="0"/>
-        <v>0.16666666666666607</v>
+        <v>0.58333333333333393</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3691,18 +4568,18 @@
         <v>43933</v>
       </c>
       <c r="D39" s="20">
-        <v>0.80902777777777779</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E39" s="23">
-        <v>0.83333333333333337</v>
+        <v>0.84375</v>
       </c>
       <c r="F39" s="34"/>
       <c r="G39" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H39" s="27">
         <f t="shared" si="0"/>
-        <v>0.58333333333333393</v>
+        <v>0.24999999999999911</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3714,18 +4591,18 @@
         <v>43933</v>
       </c>
       <c r="D40" s="20">
-        <v>0.83333333333333337</v>
+        <v>0.84444444444444444</v>
       </c>
       <c r="E40" s="23">
-        <v>0.84375</v>
+        <v>0.84583333333333333</v>
       </c>
       <c r="F40" s="34"/>
       <c r="G40" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H40" s="27">
         <f t="shared" si="0"/>
-        <v>0.24999999999999911</v>
+        <v>3.3333333333333215E-2</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3737,18 +4614,18 @@
         <v>43933</v>
       </c>
       <c r="D41" s="20">
-        <v>0.84444444444444444</v>
+        <v>0.84583333333333333</v>
       </c>
       <c r="E41" s="23">
-        <v>0.84583333333333333</v>
+        <v>0.85069444444444453</v>
       </c>
       <c r="F41" s="34"/>
       <c r="G41" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H41" s="27">
         <f t="shared" si="0"/>
-        <v>3.3333333333333215E-2</v>
+        <v>0.11666666666666892</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3760,18 +4637,18 @@
         <v>43933</v>
       </c>
       <c r="D42" s="20">
-        <v>0.84583333333333333</v>
+        <v>0.85069444444444453</v>
       </c>
       <c r="E42" s="23">
-        <v>0.85069444444444453</v>
+        <v>0.85763888888888884</v>
       </c>
       <c r="F42" s="34"/>
       <c r="G42" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H42" s="27">
         <f t="shared" si="0"/>
-        <v>0.11666666666666892</v>
+        <v>0.16666666666666341</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3783,18 +4660,18 @@
         <v>43933</v>
       </c>
       <c r="D43" s="20">
-        <v>0.85069444444444453</v>
+        <v>0.85763888888888884</v>
       </c>
       <c r="E43" s="23">
-        <v>0.85763888888888884</v>
+        <v>0.86458333333333337</v>
       </c>
       <c r="F43" s="34"/>
       <c r="G43" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H43" s="27">
         <f t="shared" si="0"/>
-        <v>0.16666666666666341</v>
+        <v>0.16666666666666874</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3806,18 +4683,18 @@
         <v>43933</v>
       </c>
       <c r="D44" s="20">
-        <v>0.85763888888888884</v>
+        <v>0.86458333333333337</v>
       </c>
       <c r="E44" s="23">
-        <v>0.86458333333333337</v>
+        <v>0.86805555555555547</v>
       </c>
       <c r="F44" s="34"/>
       <c r="G44" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H44" s="27">
         <f t="shared" si="0"/>
-        <v>0.16666666666666874</v>
+        <v>8.3333333333330373E-2</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3826,13 +4703,13 @@
         <v>6977</v>
       </c>
       <c r="C45" s="22">
-        <v>43933</v>
+        <v>43936</v>
       </c>
       <c r="D45" s="20">
-        <v>0.86458333333333337</v>
+        <v>0.89236111111111116</v>
       </c>
       <c r="E45" s="23">
-        <v>0.86805555555555547</v>
+        <v>0.89583333333333337</v>
       </c>
       <c r="F45" s="34"/>
       <c r="G45" s="17" t="s">
@@ -3840,7 +4717,7 @@
       </c>
       <c r="H45" s="27">
         <f t="shared" si="0"/>
-        <v>8.3333333333330373E-2</v>
+        <v>8.3333333333333037E-2</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3852,18 +4729,18 @@
         <v>43936</v>
       </c>
       <c r="D46" s="20">
-        <v>0.89236111111111116</v>
+        <v>0.89583333333333337</v>
       </c>
       <c r="E46" s="23">
-        <v>0.89583333333333337</v>
+        <v>0.89930555555555547</v>
       </c>
       <c r="F46" s="34"/>
       <c r="G46" s="17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H46" s="27">
         <f t="shared" si="0"/>
-        <v>8.3333333333333037E-2</v>
+        <v>8.3333333333330373E-2</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3875,10 +4752,10 @@
         <v>43936</v>
       </c>
       <c r="D47" s="20">
-        <v>0.89583333333333337</v>
+        <v>0.89930555555555547</v>
       </c>
       <c r="E47" s="23">
-        <v>0.89930555555555547</v>
+        <v>0.90625</v>
       </c>
       <c r="F47" s="34"/>
       <c r="G47" s="17" t="s">
@@ -3886,7 +4763,7 @@
       </c>
       <c r="H47" s="27">
         <f t="shared" si="0"/>
-        <v>8.3333333333330373E-2</v>
+        <v>0.16666666666666874</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3895,21 +4772,21 @@
         <v>6977</v>
       </c>
       <c r="C48" s="22">
-        <v>43936</v>
+        <v>43937</v>
       </c>
       <c r="D48" s="20">
-        <v>0.89930555555555547</v>
+        <v>0.17013888888888887</v>
       </c>
       <c r="E48" s="23">
-        <v>0.90625</v>
+        <v>0.17500000000000002</v>
       </c>
       <c r="F48" s="34"/>
       <c r="G48" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H48" s="27">
         <f t="shared" si="0"/>
-        <v>0.16666666666666874</v>
+        <v>0.11666666666666758</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3921,18 +4798,18 @@
         <v>43937</v>
       </c>
       <c r="D49" s="20">
-        <v>0.17013888888888887</v>
+        <v>0.17500000000000002</v>
       </c>
       <c r="E49" s="23">
-        <v>0.17500000000000002</v>
+        <v>0.21111111111111111</v>
       </c>
       <c r="F49" s="34"/>
       <c r="G49" s="17" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="H49" s="27">
         <f t="shared" si="0"/>
-        <v>0.11666666666666758</v>
+        <v>0.86666666666666625</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3944,10 +4821,10 @@
         <v>43937</v>
       </c>
       <c r="D50" s="20">
-        <v>0.17500000000000002</v>
+        <v>0.21111111111111111</v>
       </c>
       <c r="E50" s="23">
-        <v>0.21111111111111111</v>
+        <v>0.21944444444444444</v>
       </c>
       <c r="F50" s="34"/>
       <c r="G50" s="17" t="s">
@@ -3955,7 +4832,7 @@
       </c>
       <c r="H50" s="27">
         <f t="shared" si="0"/>
-        <v>0.86666666666666625</v>
+        <v>0.19999999999999996</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3967,28 +4844,32 @@
         <v>43937</v>
       </c>
       <c r="D51" s="20">
-        <v>0.21111111111111111</v>
-      </c>
-      <c r="E51" s="23">
-        <v>0.21527777777777779</v>
-      </c>
+        <v>0.21944444444444444</v>
+      </c>
+      <c r="E51" s="23"/>
       <c r="F51" s="34"/>
       <c r="G51" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H51" s="27">
         <f t="shared" si="0"/>
-        <v>0.10000000000000031</v>
+        <v>-5.2666666666666666</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="33"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="22"/>
+      <c r="B52" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C52" s="22">
+        <v>43937</v>
+      </c>
       <c r="D52" s="20"/>
       <c r="E52" s="23"/>
       <c r="F52" s="34"/>
-      <c r="G52" s="17"/>
+      <c r="G52" s="17" t="s">
+        <v>61</v>
+      </c>
       <c r="H52" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3996,12 +4877,18 @@
     </row>
     <row r="53" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="33"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="22"/>
+      <c r="B53" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C53" s="22">
+        <v>43937</v>
+      </c>
       <c r="D53" s="20"/>
       <c r="E53" s="23"/>
       <c r="F53" s="34"/>
-      <c r="G53" s="17"/>
+      <c r="G53" s="17" t="s">
+        <v>59</v>
+      </c>
       <c r="H53" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4009,12 +4896,18 @@
     </row>
     <row r="54" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="33"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="22"/>
+      <c r="B54" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C54" s="22">
+        <v>43937</v>
+      </c>
       <c r="D54" s="20"/>
       <c r="E54" s="23"/>
       <c r="F54" s="34"/>
-      <c r="G54" s="17"/>
+      <c r="G54" s="17" t="s">
+        <v>60</v>
+      </c>
       <c r="H54" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4022,12 +4915,18 @@
     </row>
     <row r="55" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="33"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="22"/>
+      <c r="B55" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C55" s="22">
+        <v>43937</v>
+      </c>
       <c r="D55" s="20"/>
       <c r="E55" s="23"/>
       <c r="F55" s="34"/>
-      <c r="G55" s="17"/>
+      <c r="G55" s="17" t="s">
+        <v>62</v>
+      </c>
       <c r="H55" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4035,12 +4934,18 @@
     </row>
     <row r="56" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="33"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="22"/>
+      <c r="B56" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C56" s="22">
+        <v>43937</v>
+      </c>
       <c r="D56" s="20"/>
       <c r="E56" s="23"/>
       <c r="F56" s="34"/>
-      <c r="G56" s="17"/>
+      <c r="G56" s="17" t="s">
+        <v>63</v>
+      </c>
       <c r="H56" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4048,12 +4953,18 @@
     </row>
     <row r="57" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="33"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="22"/>
+      <c r="B57" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C57" s="22">
+        <v>43937</v>
+      </c>
       <c r="D57" s="20"/>
       <c r="E57" s="23"/>
       <c r="F57" s="34"/>
-      <c r="G57" s="17"/>
+      <c r="G57" s="17" t="s">
+        <v>63</v>
+      </c>
       <c r="H57" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4061,8 +4972,12 @@
     </row>
     <row r="58" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="33"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="22"/>
+      <c r="B58" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C58" s="22">
+        <v>43937</v>
+      </c>
       <c r="D58" s="20"/>
       <c r="E58" s="23"/>
       <c r="F58" s="34"/>
@@ -4336,7 +5251,7 @@
       <c r="F79" s="41"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>16.733333333333334</v>
+        <v>11.566666666666663</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Compiled on ModelSim and Quartus. Exported transcript files into Documentation folder
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B145391-FFBE-41B7-95C8-29DCAD8C45F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9213DCE-D3BD-4A8E-A763-A34DA0CC8B2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="128">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -255,27 +255,9 @@
     <t>Read feedback comments from part 1. -DONE</t>
   </si>
   <si>
-    <t>Pulled changes from Github. Verifying changes team members have made to .vhd files in the past few days. -DONE</t>
-  </si>
-  <si>
     <t>Compiled all project files on ModelSim and Quartus to verify it compiles. -DONE</t>
   </si>
   <si>
-    <t>Verified that all synthesised circuits are correct and looks good. -DONE</t>
-  </si>
-  <si>
-    <t>Verified that all timing simulations are correct and looks good. -DONE</t>
-  </si>
-  <si>
-    <t>Verfied that all functional simulations are correct and looks good. -DONE</t>
-  </si>
-  <si>
-    <t>Rewrite SLL64.vhd, SRA64.vhd and SRL64.vhd for better readiability. -DONE</t>
-  </si>
-  <si>
-    <t>Added documentation on VHDL interface for barrel shifters into Google Doc. -DONE</t>
-  </si>
-  <si>
     <t>Fixed obvious compilation errors. Rest of compilation errors will be dealt with tomorrow. Pushed changes before going to sleep. -NOT DONE</t>
   </si>
   <si>
@@ -472,6 +454,18 @@
   </si>
   <si>
     <t>Last attempt of submission to Canvas. DONE</t>
+  </si>
+  <si>
+    <t>Verified changes team members have made to .vhd files in the past few days. -DONE</t>
+  </si>
+  <si>
+    <t>Verfied functional simulations on ModelSim and sythesised circuits are correct and looks good. -DONE</t>
+  </si>
+  <si>
+    <t>Rewrote all .vhd files for better readability. Recompiled on ModelSim and Quartus. -DONE</t>
+  </si>
+  <si>
+    <t>Checked that all functional simulations on ModelSim are still correct and good. -DONE</t>
   </si>
 </sst>
 </file>
@@ -1378,7 +1372,7 @@
       </c>
       <c r="F6" s="32"/>
       <c r="G6" s="16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H6" s="12">
         <f t="shared" ref="H6" si="0">(E6-D6)*24</f>
@@ -1402,7 +1396,7 @@
       </c>
       <c r="F7" s="34"/>
       <c r="G7" s="17" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="H7" s="27">
         <f>(E7-D7)*24</f>
@@ -1425,7 +1419,7 @@
       </c>
       <c r="F8" s="34"/>
       <c r="G8" s="17" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="H8" s="27">
         <f t="shared" ref="H8:H71" si="1">(E8-D8)*24</f>
@@ -1448,7 +1442,7 @@
       </c>
       <c r="F9" s="34"/>
       <c r="G9" s="17" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H9" s="27">
         <f t="shared" si="1"/>
@@ -1471,7 +1465,7 @@
       </c>
       <c r="F10" s="34"/>
       <c r="G10" s="17" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="H10" s="27">
         <f t="shared" si="1"/>
@@ -1494,7 +1488,7 @@
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="17" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H11" s="27">
         <f t="shared" si="1"/>
@@ -1517,7 +1511,7 @@
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="17" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="H12" s="27">
         <f t="shared" si="1"/>
@@ -1540,7 +1534,7 @@
       </c>
       <c r="F13" s="34"/>
       <c r="G13" s="17" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="H13" s="27">
         <f t="shared" si="1"/>
@@ -1563,7 +1557,7 @@
       </c>
       <c r="F14" s="34"/>
       <c r="G14" s="17" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H14" s="27">
         <f t="shared" si="1"/>
@@ -1586,7 +1580,7 @@
       </c>
       <c r="F15" s="34"/>
       <c r="G15" s="17" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H15" s="27">
         <f t="shared" si="1"/>
@@ -1609,7 +1603,7 @@
       </c>
       <c r="F16" s="34"/>
       <c r="G16" s="17" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="H16" s="27">
         <f t="shared" si="1"/>
@@ -1632,7 +1626,7 @@
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="17" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H17" s="27">
         <f t="shared" si="1"/>
@@ -1655,7 +1649,7 @@
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="17" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H18" s="27">
         <f t="shared" si="1"/>
@@ -1678,7 +1672,7 @@
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="17" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="H19" s="27">
         <f t="shared" si="1"/>
@@ -1701,7 +1695,7 @@
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="17" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="H20" s="27">
         <f t="shared" si="1"/>
@@ -1724,7 +1718,7 @@
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="17" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="H21" s="27">
         <f t="shared" si="1"/>
@@ -1747,7 +1741,7 @@
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="17" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H22" s="27">
         <f t="shared" si="1"/>
@@ -1770,7 +1764,7 @@
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="17" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H23" s="27">
         <f t="shared" si="1"/>
@@ -1793,7 +1787,7 @@
       </c>
       <c r="F24" s="34"/>
       <c r="G24" s="17" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H24" s="27">
         <f t="shared" si="1"/>
@@ -1816,7 +1810,7 @@
       </c>
       <c r="F25" s="34"/>
       <c r="G25" s="17" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H25" s="27">
         <f t="shared" si="1"/>
@@ -1839,7 +1833,7 @@
       </c>
       <c r="F26" s="34"/>
       <c r="G26" s="17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H26" s="27">
         <f t="shared" si="1"/>
@@ -1862,7 +1856,7 @@
       </c>
       <c r="F27" s="34"/>
       <c r="G27" s="17" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="H27" s="27">
         <f t="shared" si="1"/>
@@ -1885,7 +1879,7 @@
       </c>
       <c r="F28" s="34"/>
       <c r="G28" s="17" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="H28" s="27">
         <f t="shared" si="1"/>
@@ -1908,7 +1902,7 @@
       </c>
       <c r="F29" s="34"/>
       <c r="G29" s="17" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="H29" s="27">
         <f t="shared" si="1"/>
@@ -1931,7 +1925,7 @@
       </c>
       <c r="F30" s="34"/>
       <c r="G30" s="17" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="H30" s="27">
         <f t="shared" si="1"/>
@@ -1954,7 +1948,7 @@
       </c>
       <c r="F31" s="34"/>
       <c r="G31" s="17" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="H31" s="27">
         <f t="shared" si="1"/>
@@ -1977,7 +1971,7 @@
       </c>
       <c r="F32" s="34"/>
       <c r="G32" s="17" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="H32" s="27">
         <f t="shared" si="1"/>
@@ -2000,7 +1994,7 @@
       </c>
       <c r="F33" s="34"/>
       <c r="G33" s="17" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="H33" s="27">
         <f t="shared" si="1"/>
@@ -2023,7 +2017,7 @@
       </c>
       <c r="F34" s="34"/>
       <c r="G34" s="17" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H34" s="27">
         <f t="shared" si="1"/>
@@ -2046,7 +2040,7 @@
       </c>
       <c r="F35" s="34"/>
       <c r="G35" s="17" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H35" s="27">
         <f t="shared" si="1"/>
@@ -2069,7 +2063,7 @@
       </c>
       <c r="F36" s="34"/>
       <c r="G36" s="17" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H36" s="27">
         <f t="shared" si="1"/>
@@ -2092,7 +2086,7 @@
       </c>
       <c r="F37" s="34"/>
       <c r="G37" s="17" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="H37" s="27">
         <f t="shared" si="1"/>
@@ -2115,7 +2109,7 @@
       </c>
       <c r="F38" s="34"/>
       <c r="G38" s="17" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="H38" s="27">
         <f t="shared" si="1"/>
@@ -2138,7 +2132,7 @@
       </c>
       <c r="F39" s="34"/>
       <c r="G39" s="17" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="H39" s="27">
         <f t="shared" si="1"/>
@@ -2161,7 +2155,7 @@
       </c>
       <c r="F40" s="34"/>
       <c r="G40" s="17" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H40" s="27">
         <f t="shared" si="1"/>
@@ -2184,7 +2178,7 @@
       </c>
       <c r="F41" s="34"/>
       <c r="G41" s="17" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H41" s="27">
         <f t="shared" si="1"/>
@@ -2207,7 +2201,7 @@
       </c>
       <c r="F42" s="34"/>
       <c r="G42" s="17" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="H42" s="27">
         <f t="shared" si="1"/>
@@ -2230,7 +2224,7 @@
       </c>
       <c r="F43" s="34"/>
       <c r="G43" s="17" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="H43" s="27">
         <f t="shared" si="1"/>
@@ -2253,7 +2247,7 @@
       </c>
       <c r="F44" s="34"/>
       <c r="G44" s="17" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="H44" s="27">
         <f t="shared" si="1"/>
@@ -2276,7 +2270,7 @@
       </c>
       <c r="F45" s="34"/>
       <c r="G45" s="17" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H45" s="27">
         <f t="shared" si="1"/>
@@ -2299,7 +2293,7 @@
       </c>
       <c r="F46" s="34"/>
       <c r="G46" s="17" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="H46" s="27">
         <f t="shared" si="1"/>
@@ -2322,7 +2316,7 @@
       </c>
       <c r="F47" s="34"/>
       <c r="G47" s="17" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="H47" s="27">
         <f t="shared" si="1"/>
@@ -2345,7 +2339,7 @@
       </c>
       <c r="F48" s="34"/>
       <c r="G48" s="17" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="H48" s="27">
         <f t="shared" si="1"/>
@@ -2368,7 +2362,7 @@
       </c>
       <c r="F49" s="34"/>
       <c r="G49" s="17" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="H49" s="27">
         <f t="shared" si="1"/>
@@ -2391,7 +2385,7 @@
       </c>
       <c r="F50" s="34"/>
       <c r="G50" s="17" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="H50" s="27">
         <f t="shared" si="1"/>
@@ -2414,7 +2408,7 @@
       </c>
       <c r="F51" s="34"/>
       <c r="G51" s="17" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="H51" s="27">
         <f t="shared" si="1"/>
@@ -2437,7 +2431,7 @@
       </c>
       <c r="F52" s="34"/>
       <c r="G52" s="17" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="H52" s="27">
         <f t="shared" si="1"/>
@@ -2460,7 +2454,7 @@
       </c>
       <c r="F53" s="34"/>
       <c r="G53" s="17" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="H53" s="27">
         <f t="shared" si="1"/>
@@ -2483,7 +2477,7 @@
       </c>
       <c r="F54" s="34"/>
       <c r="G54" s="17" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H54" s="27">
         <f t="shared" si="1"/>
@@ -2506,7 +2500,7 @@
       </c>
       <c r="F55" s="34"/>
       <c r="G55" s="17" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="H55" s="27">
         <f t="shared" si="1"/>
@@ -2529,7 +2523,7 @@
       </c>
       <c r="F56" s="34"/>
       <c r="G56" s="17" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="H56" s="27">
         <f t="shared" si="1"/>
@@ -2552,7 +2546,7 @@
       </c>
       <c r="F57" s="34"/>
       <c r="G57" s="17" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="H57" s="27">
         <f t="shared" si="1"/>
@@ -2575,7 +2569,7 @@
       </c>
       <c r="F58" s="34"/>
       <c r="G58" s="17" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H58" s="27">
         <f t="shared" si="1"/>
@@ -2598,7 +2592,7 @@
       </c>
       <c r="F59" s="34"/>
       <c r="G59" s="17" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="H59" s="27">
         <f t="shared" si="1"/>
@@ -2621,7 +2615,7 @@
       </c>
       <c r="F60" s="34"/>
       <c r="G60" s="17" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H60" s="27">
         <f t="shared" si="1"/>
@@ -2644,7 +2638,7 @@
       </c>
       <c r="F61" s="34"/>
       <c r="G61" s="17" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="H61" s="27">
         <f t="shared" si="1"/>
@@ -2667,7 +2661,7 @@
       </c>
       <c r="F62" s="34"/>
       <c r="G62" s="17" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="H62" s="27">
         <f t="shared" si="1"/>
@@ -2690,7 +2684,7 @@
       </c>
       <c r="F63" s="34"/>
       <c r="G63" s="17" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="H63" s="27">
         <f t="shared" si="1"/>
@@ -2713,7 +2707,7 @@
       </c>
       <c r="F64" s="34"/>
       <c r="G64" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="H64" s="27">
         <f t="shared" si="1"/>
@@ -2736,7 +2730,7 @@
       </c>
       <c r="F65" s="34"/>
       <c r="G65" s="17" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H65" s="27">
         <f t="shared" si="1"/>
@@ -2759,7 +2753,7 @@
       </c>
       <c r="F66" s="34"/>
       <c r="G66" s="17" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="H66" s="27">
         <f t="shared" si="1"/>
@@ -2782,7 +2776,7 @@
       </c>
       <c r="F67" s="34"/>
       <c r="G67" s="17" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H67" s="27">
         <f t="shared" si="1"/>
@@ -2805,7 +2799,7 @@
       </c>
       <c r="F68" s="34"/>
       <c r="G68" s="17" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H68" s="27">
         <f t="shared" si="1"/>
@@ -2828,7 +2822,7 @@
       </c>
       <c r="F69" s="34"/>
       <c r="G69" s="17" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="H69" s="27">
         <f t="shared" si="1"/>
@@ -2851,7 +2845,7 @@
       </c>
       <c r="F70" s="34"/>
       <c r="G70" s="17" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="H70" s="27">
         <f t="shared" si="1"/>
@@ -2874,7 +2868,7 @@
       </c>
       <c r="F71" s="34"/>
       <c r="G71" s="17" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H71" s="27">
         <f t="shared" si="1"/>
@@ -2897,7 +2891,7 @@
       </c>
       <c r="F72" s="34"/>
       <c r="G72" s="17" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="H72" s="27">
         <f t="shared" ref="H72:H78" si="2">(E72-D72)*24</f>
@@ -3714,8 +3708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5014613-EBCB-42CE-9E22-81901AAC5CBA}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4299,7 +4293,7 @@
       </c>
       <c r="F27" s="34"/>
       <c r="G27" s="17" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H27" s="27">
         <f t="shared" si="0"/>
@@ -4805,7 +4799,7 @@
       </c>
       <c r="F49" s="34"/>
       <c r="G49" s="17" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H49" s="27">
         <f t="shared" si="0"/>
@@ -4828,7 +4822,7 @@
       </c>
       <c r="F50" s="34"/>
       <c r="G50" s="17" t="s">
-        <v>57</v>
+        <v>124</v>
       </c>
       <c r="H50" s="27">
         <f t="shared" si="0"/>
@@ -4846,14 +4840,16 @@
       <c r="D51" s="20">
         <v>0.21944444444444444</v>
       </c>
-      <c r="E51" s="23"/>
+      <c r="E51" s="23">
+        <v>0.22222222222222221</v>
+      </c>
       <c r="F51" s="34"/>
       <c r="G51" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H51" s="27">
         <f t="shared" si="0"/>
-        <v>-5.2666666666666666</v>
+        <v>6.666666666666643E-2</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -4864,15 +4860,19 @@
       <c r="C52" s="22">
         <v>43937</v>
       </c>
-      <c r="D52" s="20"/>
-      <c r="E52" s="23"/>
+      <c r="D52" s="20">
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="E52" s="23">
+        <v>0.22708333333333333</v>
+      </c>
       <c r="F52" s="34"/>
       <c r="G52" s="17" t="s">
-        <v>61</v>
+        <v>125</v>
       </c>
       <c r="H52" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.11666666666666692</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -4883,15 +4883,19 @@
       <c r="C53" s="22">
         <v>43937</v>
       </c>
-      <c r="D53" s="20"/>
-      <c r="E53" s="23"/>
+      <c r="D53" s="20">
+        <v>0.22708333333333333</v>
+      </c>
+      <c r="E53" s="23">
+        <v>0.28125</v>
+      </c>
       <c r="F53" s="34"/>
       <c r="G53" s="17" t="s">
-        <v>59</v>
+        <v>126</v>
       </c>
       <c r="H53" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -4902,15 +4906,19 @@
       <c r="C54" s="22">
         <v>43937</v>
       </c>
-      <c r="D54" s="20"/>
-      <c r="E54" s="23"/>
+      <c r="D54" s="20">
+        <v>0.28125</v>
+      </c>
+      <c r="E54" s="23">
+        <v>0.2951388888888889</v>
+      </c>
       <c r="F54" s="34"/>
       <c r="G54" s="17" t="s">
-        <v>60</v>
+        <v>127</v>
       </c>
       <c r="H54" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.33333333333333348</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -4924,9 +4932,7 @@
       <c r="D55" s="20"/>
       <c r="E55" s="23"/>
       <c r="F55" s="34"/>
-      <c r="G55" s="17" t="s">
-        <v>62</v>
-      </c>
+      <c r="G55" s="17"/>
       <c r="H55" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4943,9 +4949,7 @@
       <c r="D56" s="20"/>
       <c r="E56" s="23"/>
       <c r="F56" s="34"/>
-      <c r="G56" s="17" t="s">
-        <v>63</v>
-      </c>
+      <c r="G56" s="17"/>
       <c r="H56" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4962,9 +4966,7 @@
       <c r="D57" s="20"/>
       <c r="E57" s="23"/>
       <c r="F57" s="34"/>
-      <c r="G57" s="17" t="s">
-        <v>63</v>
-      </c>
+      <c r="G57" s="17"/>
       <c r="H57" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5251,7 +5253,7 @@
       <c r="F79" s="41"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>11.566666666666663</v>
+        <v>18.649999999999995</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5979,8 +5981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:G33"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Captured functional and timing waveform diagrams, and RTL and Post-Fit Synthesised Circuits of LogicUnit. Captured VHDL interface of most entities. Exported transcript and summary files
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9213DCE-D3BD-4A8E-A763-A34DA0CC8B2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FB86D8-637D-48D2-B8E8-540120C187E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="133">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -466,6 +466,21 @@
   </si>
   <si>
     <t>Checked that all functional simulations on ModelSim are still correct and good. -DONE</t>
+  </si>
+  <si>
+    <t>Captured raw diagrams of functional waveforms from ModelSim for LogicUnit.vhd. - DONE</t>
+  </si>
+  <si>
+    <t>Captured VHDL interface diagrams of all entities except ArithUnit.vhd (waiting on feedback from team members). -DONE</t>
+  </si>
+  <si>
+    <t>Did not like an entity naming convenction so renamed it. Recompiled and recaptured VHDL interface, RTL and Post-Fit Diagrams. -DONE</t>
+  </si>
+  <si>
+    <t>Captured raw diagrams of timing waveforms from ModelSim for LogicUnit.vhd. Exported transcript and summary files to Documentation folder for LogicUnit.vhd. -DONE</t>
+  </si>
+  <si>
+    <t>Captured RTL and Post-Fit diagrams of LogicUnit and LogicGates. -DONE</t>
   </si>
 </sst>
 </file>
@@ -3708,8 +3723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5014613-EBCB-42CE-9E22-81901AAC5CBA}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4929,13 +4944,19 @@
       <c r="C55" s="22">
         <v>43937</v>
       </c>
-      <c r="D55" s="20"/>
-      <c r="E55" s="23"/>
+      <c r="D55" s="20">
+        <v>0.2951388888888889</v>
+      </c>
+      <c r="E55" s="23">
+        <v>0.3125</v>
+      </c>
       <c r="F55" s="34"/>
-      <c r="G55" s="17"/>
+      <c r="G55" s="17" t="s">
+        <v>128</v>
+      </c>
       <c r="H55" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.41666666666666652</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -4946,13 +4967,19 @@
       <c r="C56" s="22">
         <v>43937</v>
       </c>
-      <c r="D56" s="20"/>
-      <c r="E56" s="23"/>
+      <c r="D56" s="20">
+        <v>0.3125</v>
+      </c>
+      <c r="E56" s="23">
+        <v>0.31944444444444448</v>
+      </c>
       <c r="F56" s="34"/>
-      <c r="G56" s="17"/>
+      <c r="G56" s="17" t="s">
+        <v>129</v>
+      </c>
       <c r="H56" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.16666666666666741</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -4963,13 +4990,19 @@
       <c r="C57" s="22">
         <v>43937</v>
       </c>
-      <c r="D57" s="20"/>
-      <c r="E57" s="23"/>
+      <c r="D57" s="20">
+        <v>0.31944444444444448</v>
+      </c>
+      <c r="E57" s="23">
+        <v>0.3298611111111111</v>
+      </c>
       <c r="F57" s="34"/>
-      <c r="G57" s="17"/>
+      <c r="G57" s="17" t="s">
+        <v>132</v>
+      </c>
       <c r="H57" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.24999999999999911</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -4980,39 +5013,63 @@
       <c r="C58" s="22">
         <v>43937</v>
       </c>
-      <c r="D58" s="20"/>
-      <c r="E58" s="23"/>
+      <c r="D58" s="20">
+        <v>0.3298611111111111</v>
+      </c>
+      <c r="E58" s="23">
+        <v>0.34722222222222227</v>
+      </c>
       <c r="F58" s="34"/>
-      <c r="G58" s="17"/>
+      <c r="G58" s="17" t="s">
+        <v>130</v>
+      </c>
       <c r="H58" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.41666666666666785</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="33"/>
-      <c r="B59" s="14"/>
-      <c r="C59" s="22"/>
-      <c r="D59" s="20"/>
-      <c r="E59" s="23"/>
+      <c r="B59" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C59" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D59" s="20">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="E59" s="23">
+        <v>0.3611111111111111</v>
+      </c>
       <c r="F59" s="34"/>
-      <c r="G59" s="17"/>
+      <c r="G59" s="17" t="s">
+        <v>131</v>
+      </c>
       <c r="H59" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.33333333333333215</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="33"/>
-      <c r="B60" s="14"/>
-      <c r="C60" s="22"/>
-      <c r="D60" s="20"/>
-      <c r="E60" s="23"/>
+      <c r="B60" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C60" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D60" s="20">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="E60" s="23">
+        <v>0.36805555555555558</v>
+      </c>
       <c r="F60" s="34"/>
       <c r="G60" s="17"/>
       <c r="H60" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.16666666666666741</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5253,7 +5310,7 @@
       <c r="F79" s="41"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>18.649999999999995</v>
+        <v>20.399999999999999</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5968,7 +6025,7 @@
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="H6:H78">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7735,7 +7792,7 @@
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="H6:H78">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added cover page to report
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FB86D8-637D-48D2-B8E8-540120C187E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A24358-5457-4745-84FE-5ACA3860B1DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="137">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -477,10 +477,22 @@
     <t>Did not like an entity naming convenction so renamed it. Recompiled and recaptured VHDL interface, RTL and Post-Fit Diagrams. -DONE</t>
   </si>
   <si>
-    <t>Captured raw diagrams of timing waveforms from ModelSim for LogicUnit.vhd. Exported transcript and summary files to Documentation folder for LogicUnit.vhd. -DONE</t>
-  </si>
-  <si>
     <t>Captured RTL and Post-Fit diagrams of LogicUnit and LogicGates. -DONE</t>
+  </si>
+  <si>
+    <t>Captured raw diagrams of timing waveforms from ModelSim for LogicUnit.vhd. -DONE</t>
+  </si>
+  <si>
+    <t>Exported transcript and summary files to Documentation folder for LogicUnit.vhd. -DONE</t>
+  </si>
+  <si>
+    <t>Pushed changes to GitHub. Communicated progress made. Retiring for the "night". -DONE</t>
+  </si>
+  <si>
+    <t>6977`</t>
+  </si>
+  <si>
+    <t>Started writing the report for LogicUnit and LogicGates. Too tired to continue-NOT DONE.</t>
   </si>
 </sst>
 </file>
@@ -911,6 +923,9 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -925,9 +940,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -981,10 +993,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1307,42 +1315,42 @@
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38" t="s">
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
     </row>
     <row r="2" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="39">
+      <c r="B2" s="40">
         <v>301226977</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
     </row>
     <row r="3" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
     </row>
     <row r="4" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" s="1" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3723,8 +3731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5014613-EBCB-42CE-9E22-81901AAC5CBA}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3744,42 +3752,42 @@
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38" t="s">
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
     </row>
     <row r="2" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="39">
+      <c r="B2" s="40">
         <v>301226977</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
     </row>
     <row r="3" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
     </row>
     <row r="4" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" s="1" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4998,7 +5006,7 @@
       </c>
       <c r="F57" s="34"/>
       <c r="G57" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H57" s="27">
         <f t="shared" si="0"/>
@@ -5040,15 +5048,15 @@
         <v>0.34722222222222227</v>
       </c>
       <c r="E59" s="23">
-        <v>0.3611111111111111</v>
+        <v>0.3576388888888889</v>
       </c>
       <c r="F59" s="34"/>
       <c r="G59" s="17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H59" s="27">
         <f t="shared" si="0"/>
-        <v>0.33333333333333215</v>
+        <v>0.24999999999999911</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5060,42 +5068,64 @@
         <v>43937</v>
       </c>
       <c r="D60" s="20">
+        <v>0.3576388888888889</v>
+      </c>
+      <c r="E60" s="23">
         <v>0.3611111111111111</v>
       </c>
-      <c r="E60" s="23">
-        <v>0.36805555555555558</v>
-      </c>
       <c r="F60" s="34"/>
-      <c r="G60" s="17"/>
+      <c r="G60" s="17" t="s">
+        <v>133</v>
+      </c>
       <c r="H60" s="27">
         <f t="shared" si="0"/>
-        <v>0.16666666666666741</v>
+        <v>8.3333333333333037E-2</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="33"/>
-      <c r="B61" s="14"/>
-      <c r="C61" s="22"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="23"/>
+      <c r="B61" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C61" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D61" s="20">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="E61" s="23">
+        <v>0.36805555555555558</v>
+      </c>
       <c r="F61" s="34"/>
-      <c r="G61" s="17"/>
+      <c r="G61" s="17" t="s">
+        <v>136</v>
+      </c>
       <c r="H61" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.16666666666666741</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="33"/>
-      <c r="B62" s="14"/>
-      <c r="C62" s="22"/>
-      <c r="D62" s="20"/>
-      <c r="E62" s="23"/>
+      <c r="B62" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C62" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D62" s="20">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="E62" s="23">
+        <v>0.37152777777777773</v>
+      </c>
       <c r="F62" s="34"/>
-      <c r="G62" s="17"/>
+      <c r="G62" s="17" t="s">
+        <v>134</v>
+      </c>
       <c r="H62" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3333333333331705E-2</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5198,7 +5228,7 @@
       <c r="F70" s="34"/>
       <c r="G70" s="17"/>
       <c r="H70" s="27">
-        <f t="shared" ref="H70:H129" si="1">(E70-D70)*24</f>
+        <f t="shared" ref="H70:H78" si="1">(E70-D70)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -5307,10 +5337,10 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F79" s="41"/>
+      <c r="F79" s="37"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>20.399999999999999</v>
+        <v>20.483333333333331</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6059,42 +6089,42 @@
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38" t="s">
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
     </row>
     <row r="2" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="39">
+      <c r="B2" s="40">
         <v>301226977</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
     </row>
     <row r="3" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
     </row>
     <row r="4" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" s="1" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Discovered Quartus' bird's eye view. Recaptured diagrams for LogicUnit
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A24358-5457-4745-84FE-5ACA3860B1DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE3A3FB-6C5A-468B-A330-7C9312CFB3FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="138">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -489,10 +489,13 @@
     <t>Pushed changes to GitHub. Communicated progress made. Retiring for the "night". -DONE</t>
   </si>
   <si>
-    <t>6977`</t>
-  </si>
-  <si>
     <t>Started writing the report for LogicUnit and LogicGates. Too tired to continue-NOT DONE.</t>
+  </si>
+  <si>
+    <t>Read changes made by team members and verified that everything still works. -DONE</t>
+  </si>
+  <si>
+    <t>Discovered Quartus's Birds Eye View. Redid LogicUnit's RTL and PostFit diagrams. -DONE</t>
   </si>
 </sst>
 </file>
@@ -3731,7 +3734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5014613-EBCB-42CE-9E22-81901AAC5CBA}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
@@ -5098,7 +5101,7 @@
       </c>
       <c r="F61" s="34"/>
       <c r="G61" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H61" s="27">
         <f t="shared" si="0"/>
@@ -5107,8 +5110,8 @@
     </row>
     <row r="62" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="33"/>
-      <c r="B62" s="14" t="s">
-        <v>135</v>
+      <c r="B62" s="14">
+        <v>6977</v>
       </c>
       <c r="C62" s="22">
         <v>43937</v>
@@ -5130,28 +5133,48 @@
     </row>
     <row r="63" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="33"/>
-      <c r="B63" s="14"/>
-      <c r="C63" s="22"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="23"/>
+      <c r="B63" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C63" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D63" s="20">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="E63" s="23">
+        <v>0.89583333333333337</v>
+      </c>
       <c r="F63" s="34"/>
-      <c r="G63" s="17"/>
+      <c r="G63" s="17" t="s">
+        <v>136</v>
+      </c>
       <c r="H63" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.16666666666666874</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="33"/>
-      <c r="B64" s="14"/>
-      <c r="C64" s="22"/>
-      <c r="D64" s="20"/>
-      <c r="E64" s="23"/>
+      <c r="B64" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C64" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D64" s="20">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="E64" s="23">
+        <v>0.92361111111111116</v>
+      </c>
       <c r="F64" s="34"/>
-      <c r="G64" s="17"/>
+      <c r="G64" s="17" t="s">
+        <v>137</v>
+      </c>
       <c r="H64" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.66666666666666696</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5340,7 +5363,7 @@
       <c r="F79" s="37"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>20.483333333333331</v>
+        <v>21.316666666666666</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added transcript and summary files, and RTL and Post-Fit Diagrams for ArithUnit and Adder
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE3A3FB-6C5A-468B-A330-7C9312CFB3FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98163258-01D1-448D-AEE0-983C06E20516}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="140">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -496,6 +496,12 @@
   </si>
   <si>
     <t>Discovered Quartus's Birds Eye View. Redid LogicUnit's RTL and PostFit diagrams. -DONE</t>
+  </si>
+  <si>
+    <t>Exported transcript and summary files to Documentation folder for ArithUnit.vhd. -DONE</t>
+  </si>
+  <si>
+    <t>Captured raw diagrams of RTL and Post-Fit diagrams of ArithUnit and Adder. -DONE</t>
   </si>
 </sst>
 </file>
@@ -3734,8 +3740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5014613-EBCB-42CE-9E22-81901AAC5CBA}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5179,28 +5185,48 @@
     </row>
     <row r="65" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="33"/>
-      <c r="B65" s="14"/>
-      <c r="C65" s="22"/>
-      <c r="D65" s="20"/>
-      <c r="E65" s="23"/>
+      <c r="B65" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C65" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D65" s="20">
+        <v>0.92361111111111116</v>
+      </c>
+      <c r="E65" s="23">
+        <v>0.93402777777777779</v>
+      </c>
       <c r="F65" s="34"/>
-      <c r="G65" s="17"/>
+      <c r="G65" s="17" t="s">
+        <v>138</v>
+      </c>
       <c r="H65" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.24999999999999911</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="33"/>
-      <c r="B66" s="14"/>
-      <c r="C66" s="22"/>
-      <c r="D66" s="20"/>
-      <c r="E66" s="23"/>
+      <c r="B66" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C66" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D66" s="20">
+        <v>0.93402777777777779</v>
+      </c>
+      <c r="E66" s="23">
+        <v>0.96180555555555547</v>
+      </c>
       <c r="F66" s="34"/>
-      <c r="G66" s="17"/>
+      <c r="G66" s="17" t="s">
+        <v>139</v>
+      </c>
       <c r="H66" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.6666666666666643</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5363,7 +5389,7 @@
       <c r="F79" s="37"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>21.316666666666666</v>
+        <v>22.233333333333331</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Exported transcript and waveform images for ArithUnit. Compiled on ModelSim and Quartus.
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98163258-01D1-448D-AEE0-983C06E20516}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0FA7F7-1CE7-4002-9156-16E5275B01BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="141">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -502,6 +502,9 @@
   </si>
   <si>
     <t>Captured raw diagrams of RTL and Post-Fit diagrams of ArithUnit and Adder. -DONE</t>
+  </si>
+  <si>
+    <t>Captured raw diagrams of functional and timing waveforms from ModelSim for ArithUnit.vhd. - DONE</t>
   </si>
 </sst>
 </file>
@@ -3741,7 +3744,7 @@
   <dimension ref="A1:I782"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5231,15 +5234,25 @@
     </row>
     <row r="67" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="33"/>
-      <c r="B67" s="14"/>
-      <c r="C67" s="22"/>
-      <c r="D67" s="20"/>
-      <c r="E67" s="23"/>
+      <c r="B67" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C67" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D67" s="20">
+        <v>0.96180555555555547</v>
+      </c>
+      <c r="E67" s="23">
+        <v>0.99930555555555556</v>
+      </c>
       <c r="F67" s="34"/>
-      <c r="G67" s="17"/>
+      <c r="G67" s="17" t="s">
+        <v>140</v>
+      </c>
       <c r="H67" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.90000000000000213</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5389,7 +5402,7 @@
       <c r="F79" s="37"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>22.233333333333331</v>
+        <v>23.133333333333333</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed an issue where .sdo and .vdo for ExecUnit was not updated properly
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0FA7F7-1CE7-4002-9156-16E5275B01BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2260BA-4B01-4C01-8D86-85FB0C1A9FAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="143">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -504,7 +504,13 @@
     <t>Captured raw diagrams of RTL and Post-Fit diagrams of ArithUnit and Adder. -DONE</t>
   </si>
   <si>
-    <t>Captured raw diagrams of functional and timing waveforms from ModelSim for ArithUnit.vhd. - DONE</t>
+    <t>Captured raw diagrams of functional and timing waveforms from ModelSim for ArithUnit.vhd.  - DONE</t>
+  </si>
+  <si>
+    <t>Added more raw diagrams of functional waveforms from  ModelSim for ExecUnit.vhd. Taking a small break.  - DONE</t>
+  </si>
+  <si>
+    <t>Discovered wrong results while capturing timing waveforms for ExecUnit.vhd. Issue was .sdo and .vho files for ExecUnit were not updated. Fixed issue by recompiling on Quartus. -DONE</t>
   </si>
 </sst>
 </file>
@@ -1306,7 +1312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090E6E40-83BD-4CBB-97D3-102021CD8368}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A58" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G65" sqref="A65:G74"/>
     </sheetView>
   </sheetViews>
@@ -3743,8 +3749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5014613-EBCB-42CE-9E22-81901AAC5CBA}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5257,41 +5263,69 @@
     </row>
     <row r="68" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="33"/>
-      <c r="B68" s="14"/>
-      <c r="C68" s="22"/>
-      <c r="D68" s="20"/>
-      <c r="E68" s="23"/>
+      <c r="B68" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C68" s="22">
+        <v>43938</v>
+      </c>
+      <c r="D68" s="20">
+        <v>0</v>
+      </c>
+      <c r="E68" s="23">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="F68" s="34"/>
-      <c r="G68" s="17"/>
+      <c r="G68" s="17" t="s">
+        <v>141</v>
+      </c>
       <c r="H68" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="33"/>
-      <c r="B69" s="14"/>
-      <c r="C69" s="22"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="23"/>
+      <c r="B69" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C69" s="22">
+        <v>43938</v>
+      </c>
+      <c r="D69" s="20">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="E69" s="23">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="F69" s="34"/>
-      <c r="G69" s="17"/>
+      <c r="G69" s="17" t="s">
+        <v>142</v>
+      </c>
       <c r="H69" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.4999999999999996</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="33"/>
-      <c r="B70" s="14"/>
-      <c r="C70" s="22"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="23"/>
+      <c r="B70" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C70" s="22">
+        <v>43938</v>
+      </c>
+      <c r="D70" s="20">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E70" s="23">
+        <v>0.17708333333333334</v>
+      </c>
       <c r="F70" s="34"/>
       <c r="G70" s="17"/>
       <c r="H70" s="27">
         <f t="shared" ref="H70:H78" si="1">(E70-D70)*24</f>
-        <v>0</v>
+        <v>0.25000000000000044</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5402,7 +5436,7 @@
       <c r="F79" s="37"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>23.133333333333333</v>
+        <v>25.383333333333333</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed and updated waveforms for ExecUnit. Updated transcript files
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2260BA-4B01-4C01-8D86-85FB0C1A9FAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846C0E38-AC83-45B7-9FBA-D9A00075066E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="147">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -511,6 +511,18 @@
   </si>
   <si>
     <t>Discovered wrong results while capturing timing waveforms for ExecUnit.vhd. Issue was .sdo and .vho files for ExecUnit were not updated. Fixed issue by recompiling on Quartus. -DONE</t>
+  </si>
+  <si>
+    <t>Verified that LogicUnit behaves as expected for Timing Simultion. -DONE</t>
+  </si>
+  <si>
+    <t>Verified that timing simulation for ArithUnit and ExecUnit are still good. Communicated issue and fix to team members. Pushed changes to Github. -DONE</t>
+  </si>
+  <si>
+    <t>Discovered that test bench vector is ArithUnit01.tvs with team member. Changed it and replaced transcript files as waveforms are still valid. -DONE</t>
+  </si>
+  <si>
+    <t>Captured raw diagrams of timing waveforms from ModelSim for ExecUnit.vhd. Fixed a timing waveform in ArithUnit.vhd. -DONE</t>
   </si>
 </sst>
 </file>
@@ -1312,7 +1324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090E6E40-83BD-4CBB-97D3-102021CD8368}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G65" sqref="A65:G74"/>
     </sheetView>
   </sheetViews>
@@ -3750,7 +3762,7 @@
   <dimension ref="A1:I782"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5319,52 +5331,84 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="E70" s="23">
-        <v>0.17708333333333334</v>
+        <v>0.18055555555555555</v>
       </c>
       <c r="F70" s="34"/>
-      <c r="G70" s="17"/>
+      <c r="G70" s="17" t="s">
+        <v>144</v>
+      </c>
       <c r="H70" s="27">
         <f t="shared" ref="H70:H78" si="1">(E70-D70)*24</f>
-        <v>0.25000000000000044</v>
+        <v>0.33333333333333348</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="33"/>
-      <c r="B71" s="14"/>
-      <c r="C71" s="22"/>
-      <c r="D71" s="20"/>
-      <c r="E71" s="23"/>
+      <c r="B71" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C71" s="22">
+        <v>43938</v>
+      </c>
+      <c r="D71" s="20">
+        <v>0.18055555555555555</v>
+      </c>
+      <c r="E71" s="23">
+        <v>0.1875</v>
+      </c>
       <c r="F71" s="34"/>
-      <c r="G71" s="17"/>
+      <c r="G71" s="17" t="s">
+        <v>143</v>
+      </c>
       <c r="H71" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.16666666666666674</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="33"/>
-      <c r="B72" s="14"/>
-      <c r="C72" s="22"/>
-      <c r="D72" s="20"/>
-      <c r="E72" s="23"/>
+      <c r="B72" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C72" s="22">
+        <v>43938</v>
+      </c>
+      <c r="D72" s="20">
+        <v>0.1875</v>
+      </c>
+      <c r="E72" s="23">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="F72" s="34"/>
-      <c r="G72" s="17"/>
+      <c r="G72" s="17" t="s">
+        <v>145</v>
+      </c>
       <c r="H72" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.50000000000000022</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="33"/>
-      <c r="B73" s="14"/>
-      <c r="C73" s="22"/>
-      <c r="D73" s="20"/>
-      <c r="E73" s="23"/>
+      <c r="B73" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C73" s="22">
+        <v>43938</v>
+      </c>
+      <c r="D73" s="20">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="E73" s="23">
+        <v>0.25</v>
+      </c>
       <c r="F73" s="34"/>
-      <c r="G73" s="17"/>
+      <c r="G73" s="17" t="s">
+        <v>146</v>
+      </c>
       <c r="H73" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.99999999999999978</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5436,7 +5480,7 @@
       <c r="F79" s="37"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>25.383333333333333</v>
+        <v>27.133333333333333</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Captured RTL and Post-Fit diagrams for ShiftUnit and barrel shifters. Exported summary files to Documentation
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846C0E38-AC83-45B7-9FBA-D9A00075066E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368362B2-2A2A-4609-9AC8-0B0FDE0660FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="148">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -523,6 +523,9 @@
   </si>
   <si>
     <t>Captured raw diagrams of timing waveforms from ModelSim for ExecUnit.vhd. Fixed a timing waveform in ArithUnit.vhd. -DONE</t>
+  </si>
+  <si>
+    <t>Captured raw diagrams of RTL and Post-Fit diagrams of ShiftUnit, SLL64, SRL64 and SRA64. Exported summary files to Documentation for ShiftUnit.vhd.  -DONE</t>
   </si>
 </sst>
 </file>
@@ -3761,7 +3764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5014613-EBCB-42CE-9E22-81901AAC5CBA}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
@@ -5413,15 +5416,25 @@
     </row>
     <row r="74" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="33"/>
-      <c r="B74" s="14"/>
-      <c r="C74" s="22"/>
-      <c r="D74" s="20"/>
-      <c r="E74" s="23"/>
+      <c r="B74" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C74" s="22">
+        <v>43938</v>
+      </c>
+      <c r="D74" s="20">
+        <v>0.25</v>
+      </c>
+      <c r="E74" s="23">
+        <v>0.30902777777777779</v>
+      </c>
       <c r="F74" s="34"/>
-      <c r="G74" s="17"/>
+      <c r="G74" s="17" t="s">
+        <v>147</v>
+      </c>
       <c r="H74" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.416666666666667</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5480,7 +5493,7 @@
       <c r="F79" s="37"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>27.133333333333333</v>
+        <v>28.55</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Prepare a folder for easy submission
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368362B2-2A2A-4609-9AC8-0B0FDE0660FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89814CB8-4D39-433D-A1E6-8BF66E29151E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="150">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -526,6 +526,12 @@
   </si>
   <si>
     <t>Captured raw diagrams of RTL and Post-Fit diagrams of ShiftUnit, SLL64, SRL64 and SRA64. Exported summary files to Documentation for ShiftUnit.vhd.  -DONE</t>
+  </si>
+  <si>
+    <t>Started working on the report with feedback comments from part 1 in mind. Too tired to continue. -NOT DONE</t>
+  </si>
+  <si>
+    <t>Combined summary files into one .txt file. Prepare a folder for a quick and easy submission. Updated team members on progress and pushed to Github. Retiring for the "night". -DONE</t>
   </si>
 </sst>
 </file>
@@ -3765,7 +3771,7 @@
   <dimension ref="A1:I782"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G74" sqref="G74"/>
+      <selection activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5439,34 +5445,58 @@
     </row>
     <row r="75" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="33"/>
-      <c r="B75" s="14"/>
-      <c r="C75" s="22"/>
-      <c r="D75" s="20"/>
-      <c r="E75" s="23"/>
+      <c r="B75" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C75" s="22">
+        <v>43938</v>
+      </c>
+      <c r="D75" s="20">
+        <v>0.30902777777777779</v>
+      </c>
+      <c r="E75" s="23">
+        <v>0.35416666666666669</v>
+      </c>
       <c r="F75" s="34"/>
-      <c r="G75" s="17"/>
+      <c r="G75" s="17" t="s">
+        <v>148</v>
+      </c>
       <c r="H75" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.0833333333333335</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="33"/>
-      <c r="B76" s="14"/>
-      <c r="C76" s="22"/>
-      <c r="D76" s="20"/>
-      <c r="E76" s="23"/>
+      <c r="B76" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C76" s="22">
+        <v>43938</v>
+      </c>
+      <c r="D76" s="20">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E76" s="23">
+        <v>0.36458333333333331</v>
+      </c>
       <c r="F76" s="34"/>
-      <c r="G76" s="17"/>
+      <c r="G76" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="H76" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.24999999999999911</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="33"/>
-      <c r="B77" s="14"/>
-      <c r="C77" s="22"/>
+      <c r="B77" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C77" s="22">
+        <v>43938</v>
+      </c>
       <c r="D77" s="20"/>
       <c r="E77" s="23"/>
       <c r="F77" s="34"/>
@@ -5478,8 +5508,12 @@
     </row>
     <row r="78" spans="1:8" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="35"/>
-      <c r="B78" s="15"/>
-      <c r="C78" s="24"/>
+      <c r="B78" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C78" s="22">
+        <v>43938</v>
+      </c>
       <c r="D78" s="25"/>
       <c r="E78" s="26"/>
       <c r="F78" s="36"/>
@@ -5493,7 +5527,7 @@
       <c r="F79" s="37"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>28.55</v>
+        <v>29.883333333333333</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Worked on report. Added SHiftUnit annotated diagrams to report
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G47-6977-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalprojectpart2\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96964249-767C-46C7-AA77-79E5947ED4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D02DEA1-821D-4215-8B32-783391D9873C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="144">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -504,10 +504,16 @@
     <t>Tried to compile on ModelSim to find all compilation errors for all .vhd files. Fixed ExecUnit.vhd completely. There are still errors are other .vhd files. Retiring for the day- DONE</t>
   </si>
   <si>
-    <t>Working on the report on Google Docs. Re-capture waveform diagrams as needed to fit narrative better. Took a small break to grab some food. -NOT DONE</t>
-  </si>
-  <si>
     <t>Working on the report. -NOT DONE</t>
+  </si>
+  <si>
+    <t>Working on the report. Re-capture waveform diagrams as needed to fit narrative better. Took a small break to grab some food. -NOT DONE</t>
+  </si>
+  <si>
+    <t>Working on the report. -DONE</t>
+  </si>
+  <si>
+    <t>Final checks that submission folder is fully ready to submission. Zipped folder and submitted ZIP folder on canvas. -DONE</t>
   </si>
 </sst>
 </file>
@@ -3747,7 +3753,7 @@
   <dimension ref="A1:I782"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F68" sqref="F68"/>
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5251,7 +5257,7 @@
       </c>
       <c r="F67" s="34"/>
       <c r="G67" s="17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H67" s="27">
         <f t="shared" si="0"/>
@@ -5274,7 +5280,7 @@
       </c>
       <c r="F68" s="34"/>
       <c r="G68" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H68" s="27">
         <f t="shared" si="0"/>
@@ -5283,28 +5289,48 @@
     </row>
     <row r="69" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="33"/>
-      <c r="B69" s="14"/>
-      <c r="C69" s="22"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="23"/>
+      <c r="B69" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C69" s="22">
+        <v>43938</v>
+      </c>
+      <c r="D69" s="20">
+        <v>0.3979166666666667</v>
+      </c>
+      <c r="E69" s="23">
+        <v>0.98125000000000007</v>
+      </c>
       <c r="F69" s="34"/>
-      <c r="G69" s="17"/>
+      <c r="G69" s="17" t="s">
+        <v>142</v>
+      </c>
       <c r="H69" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="33"/>
-      <c r="B70" s="14"/>
-      <c r="C70" s="22"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="23"/>
+      <c r="B70" s="14">
+        <v>6977</v>
+      </c>
+      <c r="C70" s="22">
+        <v>43938</v>
+      </c>
+      <c r="D70" s="20">
+        <v>0.98125000000000007</v>
+      </c>
+      <c r="E70" s="23">
+        <v>0.98958333333333337</v>
+      </c>
       <c r="F70" s="34"/>
-      <c r="G70" s="17"/>
+      <c r="G70" s="17" t="s">
+        <v>143</v>
+      </c>
       <c r="H70" s="27">
         <f t="shared" ref="H70:H78" si="1">(E70-D70)*24</f>
-        <v>0</v>
+        <v>0.19999999999999929</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5415,7 +5441,7 @@
       <c r="F79" s="37"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>33.683333333333337</v>
+        <v>47.88333333333334</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>